<commit_message>
create account only with invitation and code
</commit_message>
<xml_diff>
--- a/files/onboarding/Agroassist_Plantilla_Onboarding.xlsx
+++ b/files/onboarding/Agroassist_Plantilla_Onboarding.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
-    <sheet state="hidden" name="Hoja 2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Hoja 2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nombre Cuartel</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Arandanos</t>
+  </si>
+  <si>
+    <t>Moras</t>
+  </si>
+  <si>
+    <t>Frambuesas</t>
   </si>
 </sst>
 </file>
@@ -96,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,9 +111,6 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -3573,7 +3576,7 @@
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1000">
-      <formula1>'Hoja 2'!$A$2:$A$5</formula1>
+      <formula1>'Hoja 2'!$A$2:$A$7</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -3600,27 +3603,35 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
4th initial step text fixed
</commit_message>
<xml_diff>
--- a/files/onboarding/Agroassist_Plantilla_Onboarding.xlsx
+++ b/files/onboarding/Agroassist_Plantilla_Onboarding.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nombre Cuartel</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Manzanas</t>
+  </si>
+  <si>
+    <t>Nogales</t>
+  </si>
+  <si>
+    <t>Avellanos</t>
+  </si>
+  <si>
+    <t>Almendros</t>
+  </si>
+  <si>
+    <t>Castaños</t>
   </si>
 </sst>
 </file>
@@ -108,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -116,7 +128,6 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -124,7 +135,18 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1240,2349 +1262,2354 @@
       <c r="C220" s="3"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="C221" s="5"/>
+      <c r="C221" s="3"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="C222" s="5"/>
+      <c r="C222" s="3"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="C223" s="5"/>
+      <c r="C223" s="3"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="C224" s="5"/>
+      <c r="C224" s="3"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="C225" s="5"/>
+      <c r="C225" s="3"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="C226" s="5"/>
+      <c r="C226" s="3"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="C227" s="5"/>
+      <c r="C227" s="3"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="C228" s="5"/>
+      <c r="C228" s="3"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="C229" s="5"/>
+      <c r="C229" s="3"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="C230" s="5"/>
+      <c r="C230" s="3"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="C231" s="5"/>
+      <c r="C231" s="3"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="C232" s="5"/>
+      <c r="C232" s="3"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="C233" s="5"/>
+      <c r="C233" s="3"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="C234" s="5"/>
+      <c r="C234" s="3"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="C235" s="5"/>
+      <c r="C235" s="3"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="C236" s="5"/>
+      <c r="C236" s="3"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="C237" s="5"/>
+      <c r="C237" s="3"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="C238" s="5"/>
+      <c r="C238" s="3"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="C239" s="5"/>
+      <c r="C239" s="3"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="C240" s="5"/>
+      <c r="C240" s="3"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="C241" s="5"/>
+      <c r="C241" s="3"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="C242" s="5"/>
+      <c r="C242" s="3"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="C243" s="5"/>
+      <c r="C243" s="3"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="C244" s="5"/>
+      <c r="C244" s="3"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="C245" s="5"/>
+      <c r="C245" s="3"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="C246" s="5"/>
+      <c r="C246" s="3"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="C247" s="5"/>
+      <c r="C247" s="3"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="C248" s="5"/>
+      <c r="C248" s="3"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="C249" s="5"/>
+      <c r="C249" s="3"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="C250" s="5"/>
+      <c r="C250" s="3"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="C251" s="5"/>
+      <c r="C251" s="3"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="C252" s="5"/>
+      <c r="C252" s="3"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="C253" s="5"/>
+      <c r="C253" s="3"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="C254" s="5"/>
+      <c r="C254" s="3"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="C255" s="5"/>
+      <c r="C255" s="3"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="C256" s="5"/>
+      <c r="C256" s="3"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="C257" s="5"/>
+      <c r="C257" s="3"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="C258" s="5"/>
+      <c r="C258" s="3"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="C259" s="5"/>
+      <c r="C259" s="3"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="C260" s="5"/>
+      <c r="C260" s="3"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="C261" s="5"/>
+      <c r="C261" s="3"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="C262" s="5"/>
+      <c r="C262" s="3"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="C263" s="5"/>
+      <c r="C263" s="3"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="C264" s="5"/>
+      <c r="C264" s="3"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="C265" s="5"/>
+      <c r="C265" s="3"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="C266" s="5"/>
+      <c r="C266" s="3"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="C267" s="5"/>
+      <c r="C267" s="3"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="C268" s="5"/>
+      <c r="C268" s="3"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="C269" s="5"/>
+      <c r="C269" s="3"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="C270" s="5"/>
+      <c r="C270" s="3"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="C271" s="5"/>
+      <c r="C271" s="3"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="C272" s="5"/>
+      <c r="C272" s="3"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="C273" s="5"/>
+      <c r="C273" s="3"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="C274" s="5"/>
+      <c r="C274" s="3"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="C275" s="5"/>
+      <c r="C275" s="3"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="C276" s="5"/>
+      <c r="C276" s="3"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="C277" s="5"/>
+      <c r="C277" s="3"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="C278" s="5"/>
+      <c r="C278" s="3"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="C279" s="5"/>
+      <c r="C279" s="3"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="C280" s="5"/>
+      <c r="C280" s="3"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="C281" s="5"/>
+      <c r="C281" s="3"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="C282" s="5"/>
+      <c r="C282" s="3"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="C283" s="5"/>
+      <c r="C283" s="3"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="C284" s="5"/>
+      <c r="C284" s="3"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="C285" s="5"/>
+      <c r="C285" s="3"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="C286" s="5"/>
+      <c r="C286" s="3"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="C287" s="5"/>
+      <c r="C287" s="3"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="C288" s="5"/>
+      <c r="C288" s="3"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="C289" s="5"/>
+      <c r="C289" s="3"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="C290" s="5"/>
+      <c r="C290" s="3"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="C291" s="5"/>
+      <c r="C291" s="3"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="C292" s="5"/>
+      <c r="C292" s="3"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="C293" s="5"/>
+      <c r="C293" s="3"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="C294" s="5"/>
+      <c r="C294" s="3"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="C295" s="5"/>
+      <c r="C295" s="3"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="C296" s="5"/>
+      <c r="C296" s="3"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="C297" s="5"/>
+      <c r="C297" s="3"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="C298" s="5"/>
+      <c r="C298" s="3"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="C299" s="5"/>
+      <c r="C299" s="3"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="C300" s="5"/>
+      <c r="C300" s="3"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="C301" s="5"/>
+      <c r="C301" s="3"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="C302" s="5"/>
+      <c r="C302" s="3"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="C303" s="5"/>
+      <c r="C303" s="3"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="C304" s="5"/>
+      <c r="C304" s="3"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="C305" s="5"/>
+      <c r="C305" s="3"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="C306" s="5"/>
+      <c r="C306" s="3"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="C307" s="5"/>
+      <c r="C307" s="3"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="C308" s="5"/>
+      <c r="C308" s="3"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="C309" s="5"/>
+      <c r="C309" s="3"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="C310" s="5"/>
+      <c r="C310" s="3"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="C311" s="5"/>
+      <c r="C311" s="3"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="C312" s="5"/>
+      <c r="C312" s="3"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="C313" s="5"/>
+      <c r="C313" s="3"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="C314" s="5"/>
+      <c r="C314" s="3"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="C315" s="5"/>
+      <c r="C315" s="3"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="C316" s="5"/>
+      <c r="C316" s="3"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="C317" s="5"/>
+      <c r="C317" s="3"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="C318" s="5"/>
+      <c r="C318" s="3"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="C319" s="5"/>
+      <c r="C319" s="3"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="C320" s="5"/>
+      <c r="C320" s="3"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="C321" s="5"/>
+      <c r="C321" s="3"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="C322" s="5"/>
+      <c r="C322" s="3"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="C323" s="5"/>
+      <c r="C323" s="3"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="C324" s="5"/>
+      <c r="C324" s="3"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="C325" s="5"/>
+      <c r="C325" s="3"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="C326" s="5"/>
+      <c r="C326" s="3"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="C327" s="5"/>
+      <c r="C327" s="3"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="C328" s="5"/>
+      <c r="C328" s="3"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="C329" s="5"/>
+      <c r="C329" s="3"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="C330" s="5"/>
+      <c r="C330" s="3"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="C331" s="5"/>
+      <c r="C331" s="3"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="C332" s="5"/>
+      <c r="C332" s="3"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="C333" s="5"/>
+      <c r="C333" s="3"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="C334" s="5"/>
+      <c r="C334" s="3"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="C335" s="5"/>
+      <c r="C335" s="3"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="C336" s="5"/>
+      <c r="C336" s="3"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="C337" s="5"/>
+      <c r="C337" s="3"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="C338" s="5"/>
+      <c r="C338" s="3"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="C339" s="5"/>
+      <c r="C339" s="3"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="C340" s="5"/>
+      <c r="C340" s="3"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="C341" s="5"/>
+      <c r="C341" s="3"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="C342" s="5"/>
+      <c r="C342" s="3"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="C343" s="5"/>
+      <c r="C343" s="3"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="C344" s="5"/>
+      <c r="C344" s="3"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="C345" s="5"/>
+      <c r="C345" s="3"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="C346" s="5"/>
+      <c r="C346" s="3"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="C347" s="5"/>
+      <c r="C347" s="3"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="C348" s="5"/>
+      <c r="C348" s="3"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="C349" s="5"/>
+      <c r="C349" s="3"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="C350" s="5"/>
+      <c r="C350" s="3"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="C351" s="5"/>
+      <c r="C351" s="3"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="C352" s="5"/>
+      <c r="C352" s="3"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="C353" s="5"/>
+      <c r="C353" s="3"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="C354" s="5"/>
+      <c r="C354" s="3"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="C355" s="5"/>
+      <c r="C355" s="3"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="C356" s="5"/>
+      <c r="C356" s="3"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="C357" s="5"/>
+      <c r="C357" s="3"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="C358" s="5"/>
+      <c r="C358" s="3"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="C359" s="5"/>
+      <c r="C359" s="3"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="C360" s="5"/>
+      <c r="C360" s="3"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="C361" s="5"/>
+      <c r="C361" s="3"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="C362" s="5"/>
+      <c r="C362" s="3"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="C363" s="5"/>
+      <c r="C363" s="3"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="C364" s="5"/>
+      <c r="C364" s="3"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="C365" s="5"/>
+      <c r="C365" s="3"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="C366" s="5"/>
+      <c r="C366" s="3"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="C367" s="5"/>
+      <c r="C367" s="3"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="C368" s="5"/>
+      <c r="C368" s="3"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="C369" s="5"/>
+      <c r="C369" s="3"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="C370" s="5"/>
+      <c r="C370" s="3"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="C371" s="5"/>
+      <c r="C371" s="3"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="C372" s="5"/>
+      <c r="C372" s="3"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="C373" s="5"/>
+      <c r="C373" s="3"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="C374" s="5"/>
+      <c r="C374" s="3"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="C375" s="5"/>
+      <c r="C375" s="3"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="C376" s="5"/>
+      <c r="C376" s="3"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="C377" s="5"/>
+      <c r="C377" s="3"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="C378" s="5"/>
+      <c r="C378" s="3"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="C379" s="5"/>
+      <c r="C379" s="3"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="C380" s="5"/>
+      <c r="C380" s="3"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="C381" s="5"/>
+      <c r="C381" s="3"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="C382" s="5"/>
+      <c r="C382" s="3"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="C383" s="5"/>
+      <c r="C383" s="3"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="C384" s="5"/>
+      <c r="C384" s="3"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="C385" s="5"/>
+      <c r="C385" s="3"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="C386" s="5"/>
+      <c r="C386" s="3"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="C387" s="5"/>
+      <c r="C387" s="3"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="C388" s="5"/>
+      <c r="C388" s="3"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="C389" s="5"/>
+      <c r="C389" s="3"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="C390" s="5"/>
+      <c r="C390" s="3"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="C391" s="5"/>
+      <c r="C391" s="3"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="C392" s="5"/>
+      <c r="C392" s="3"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="C393" s="5"/>
+      <c r="C393" s="3"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="C394" s="5"/>
+      <c r="C394" s="3"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="C395" s="5"/>
+      <c r="C395" s="3"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="C396" s="5"/>
+      <c r="C396" s="3"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="C397" s="5"/>
+      <c r="C397" s="3"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="C398" s="5"/>
+      <c r="C398" s="3"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="C399" s="5"/>
+      <c r="C399" s="3"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="C400" s="5"/>
+      <c r="C400" s="3"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="C401" s="5"/>
+      <c r="C401" s="3"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="C402" s="5"/>
+      <c r="C402" s="3"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="C403" s="5"/>
+      <c r="C403" s="3"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="C404" s="5"/>
+      <c r="C404" s="3"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="C405" s="5"/>
+      <c r="C405" s="3"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="C406" s="5"/>
+      <c r="C406" s="3"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="C407" s="5"/>
+      <c r="C407" s="3"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="C408" s="5"/>
+      <c r="C408" s="3"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="C409" s="5"/>
+      <c r="C409" s="3"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="C410" s="5"/>
+      <c r="C410" s="3"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="C411" s="5"/>
+      <c r="C411" s="3"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="C412" s="5"/>
+      <c r="C412" s="3"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="C413" s="5"/>
+      <c r="C413" s="3"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="C414" s="5"/>
+      <c r="C414" s="3"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="C415" s="5"/>
+      <c r="C415" s="3"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="C416" s="5"/>
+      <c r="C416" s="3"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="C417" s="5"/>
+      <c r="C417" s="3"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="C418" s="5"/>
+      <c r="C418" s="3"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="C419" s="5"/>
+      <c r="C419" s="3"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="C420" s="5"/>
+      <c r="C420" s="3"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="C421" s="5"/>
+      <c r="C421" s="3"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="C422" s="5"/>
+      <c r="C422" s="3"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="C423" s="5"/>
+      <c r="C423" s="3"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="C424" s="5"/>
+      <c r="C424" s="3"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="C425" s="5"/>
+      <c r="C425" s="3"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="C426" s="5"/>
+      <c r="C426" s="3"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="C427" s="5"/>
+      <c r="C427" s="3"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="C428" s="5"/>
+      <c r="C428" s="3"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="C429" s="5"/>
+      <c r="C429" s="3"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="C430" s="5"/>
+      <c r="C430" s="3"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="C431" s="5"/>
+      <c r="C431" s="3"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="C432" s="5"/>
+      <c r="C432" s="3"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="C433" s="5"/>
+      <c r="C433" s="3"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="C434" s="5"/>
+      <c r="C434" s="3"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="C435" s="5"/>
+      <c r="C435" s="3"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="C436" s="5"/>
+      <c r="C436" s="3"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="C437" s="5"/>
+      <c r="C437" s="3"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="C438" s="5"/>
+      <c r="C438" s="3"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="C439" s="5"/>
+      <c r="C439" s="3"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="C440" s="5"/>
+      <c r="C440" s="3"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="C441" s="5"/>
+      <c r="C441" s="3"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="C442" s="5"/>
+      <c r="C442" s="3"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="C443" s="5"/>
+      <c r="C443" s="3"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="C444" s="5"/>
+      <c r="C444" s="3"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="C445" s="5"/>
+      <c r="C445" s="3"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="C446" s="5"/>
+      <c r="C446" s="3"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="C447" s="5"/>
+      <c r="C447" s="3"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="C448" s="5"/>
+      <c r="C448" s="3"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="C449" s="5"/>
+      <c r="C449" s="3"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="C450" s="5"/>
+      <c r="C450" s="3"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="C451" s="5"/>
+      <c r="C451" s="3"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="C452" s="5"/>
+      <c r="C452" s="3"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="C453" s="5"/>
+      <c r="C453" s="3"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="C454" s="5"/>
+      <c r="C454" s="3"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="C455" s="5"/>
+      <c r="C455" s="3"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="C456" s="5"/>
+      <c r="C456" s="3"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="C457" s="5"/>
+      <c r="C457" s="3"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="C458" s="5"/>
+      <c r="C458" s="3"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="C459" s="5"/>
+      <c r="C459" s="3"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="C460" s="5"/>
+      <c r="C460" s="3"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="C461" s="5"/>
+      <c r="C461" s="3"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="C462" s="5"/>
+      <c r="C462" s="3"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="C463" s="5"/>
+      <c r="C463" s="3"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="C464" s="5"/>
+      <c r="C464" s="3"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="C465" s="5"/>
+      <c r="C465" s="3"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="C466" s="5"/>
+      <c r="C466" s="3"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="C467" s="5"/>
+      <c r="C467" s="3"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="C468" s="5"/>
+      <c r="C468" s="3"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="C469" s="5"/>
+      <c r="C469" s="3"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="C470" s="5"/>
+      <c r="C470" s="3"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="C471" s="5"/>
+      <c r="C471" s="3"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="C472" s="5"/>
+      <c r="C472" s="3"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="C473" s="5"/>
+      <c r="C473" s="3"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="C474" s="5"/>
+      <c r="C474" s="3"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="C475" s="5"/>
+      <c r="C475" s="3"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="C476" s="5"/>
+      <c r="C476" s="3"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="C477" s="5"/>
+      <c r="C477" s="3"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="C478" s="5"/>
+      <c r="C478" s="3"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="C479" s="5"/>
+      <c r="C479" s="3"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="C480" s="5"/>
+      <c r="C480" s="3"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="C481" s="5"/>
+      <c r="C481" s="3"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="C482" s="5"/>
+      <c r="C482" s="3"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="C483" s="5"/>
+      <c r="C483" s="3"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="C484" s="5"/>
+      <c r="C484" s="3"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="C485" s="5"/>
+      <c r="C485" s="3"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="C486" s="5"/>
+      <c r="C486" s="3"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="C487" s="5"/>
+      <c r="C487" s="3"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="C488" s="5"/>
+      <c r="C488" s="3"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="C489" s="5"/>
+      <c r="C489" s="3"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="C490" s="5"/>
+      <c r="C490" s="3"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="C491" s="5"/>
+      <c r="C491" s="3"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="C492" s="5"/>
+      <c r="C492" s="3"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="C493" s="5"/>
+      <c r="C493" s="3"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="C494" s="5"/>
+      <c r="C494" s="3"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="C495" s="5"/>
+      <c r="C495" s="3"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="C496" s="5"/>
+      <c r="C496" s="3"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="C497" s="5"/>
+      <c r="C497" s="3"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="C498" s="5"/>
+      <c r="C498" s="3"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="C499" s="5"/>
+      <c r="C499" s="3"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="C500" s="5"/>
+      <c r="C500" s="3"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="C501" s="5"/>
+      <c r="C501" s="3"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="C502" s="5"/>
+      <c r="C502" s="3"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="C503" s="5"/>
+      <c r="C503" s="3"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="C504" s="5"/>
+      <c r="C504" s="3"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="C505" s="5"/>
+      <c r="C505" s="3"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="C506" s="5"/>
+      <c r="C506" s="3"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="C507" s="5"/>
+      <c r="C507" s="3"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="C508" s="5"/>
+      <c r="C508" s="3"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="C509" s="5"/>
+      <c r="C509" s="3"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="C510" s="5"/>
+      <c r="C510" s="3"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="C511" s="5"/>
+      <c r="C511" s="3"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="C512" s="5"/>
+      <c r="C512" s="3"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="C513" s="5"/>
+      <c r="C513" s="3"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="C514" s="5"/>
+      <c r="C514" s="3"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="C515" s="5"/>
+      <c r="C515" s="3"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="C516" s="5"/>
+      <c r="C516" s="3"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="C517" s="5"/>
+      <c r="C517" s="3"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="C518" s="5"/>
+      <c r="C518" s="3"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="C519" s="5"/>
+      <c r="C519" s="3"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="C520" s="5"/>
+      <c r="C520" s="3"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="C521" s="5"/>
+      <c r="C521" s="3"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="C522" s="5"/>
+      <c r="C522" s="3"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="C523" s="5"/>
+      <c r="C523" s="3"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="C524" s="5"/>
+      <c r="C524" s="3"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="C525" s="5"/>
+      <c r="C525" s="3"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="C526" s="5"/>
+      <c r="C526" s="3"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="C527" s="5"/>
+      <c r="C527" s="3"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="C528" s="5"/>
+      <c r="C528" s="3"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="C529" s="5"/>
+      <c r="C529" s="3"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="C530" s="5"/>
+      <c r="C530" s="3"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="C531" s="5"/>
+      <c r="C531" s="3"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="C532" s="5"/>
+      <c r="C532" s="3"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="C533" s="5"/>
+      <c r="C533" s="3"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="C534" s="5"/>
+      <c r="C534" s="3"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="C535" s="5"/>
+      <c r="C535" s="3"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="C536" s="5"/>
+      <c r="C536" s="3"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="C537" s="5"/>
+      <c r="C537" s="3"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="C538" s="5"/>
+      <c r="C538" s="3"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="C539" s="5"/>
+      <c r="C539" s="3"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="C540" s="5"/>
+      <c r="C540" s="3"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="C541" s="5"/>
+      <c r="C541" s="3"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="C542" s="5"/>
+      <c r="C542" s="3"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="C543" s="5"/>
+      <c r="C543" s="3"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="C544" s="5"/>
+      <c r="C544" s="3"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="C545" s="5"/>
+      <c r="C545" s="3"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="C546" s="5"/>
+      <c r="C546" s="3"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="C547" s="5"/>
+      <c r="C547" s="3"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="C548" s="5"/>
+      <c r="C548" s="3"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="C549" s="5"/>
+      <c r="C549" s="3"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="C550" s="5"/>
+      <c r="C550" s="3"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="C551" s="5"/>
+      <c r="C551" s="3"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="C552" s="5"/>
+      <c r="C552" s="3"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="C553" s="5"/>
+      <c r="C553" s="3"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="C554" s="5"/>
+      <c r="C554" s="3"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="C555" s="5"/>
+      <c r="C555" s="3"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="C556" s="5"/>
+      <c r="C556" s="3"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="C557" s="5"/>
+      <c r="C557" s="3"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="C558" s="5"/>
+      <c r="C558" s="3"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="C559" s="5"/>
+      <c r="C559" s="3"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="C560" s="5"/>
+      <c r="C560" s="3"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="C561" s="5"/>
+      <c r="C561" s="3"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="C562" s="5"/>
+      <c r="C562" s="3"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="C563" s="5"/>
+      <c r="C563" s="3"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="C564" s="5"/>
+      <c r="C564" s="3"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="C565" s="5"/>
+      <c r="C565" s="3"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="C566" s="5"/>
+      <c r="C566" s="3"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="C567" s="5"/>
+      <c r="C567" s="3"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="C568" s="5"/>
+      <c r="C568" s="3"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="C569" s="5"/>
+      <c r="C569" s="3"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="C570" s="5"/>
+      <c r="C570" s="3"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="C571" s="5"/>
+      <c r="C571" s="3"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="C572" s="5"/>
+      <c r="C572" s="3"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="C573" s="5"/>
+      <c r="C573" s="3"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="C574" s="5"/>
+      <c r="C574" s="3"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="C575" s="5"/>
+      <c r="C575" s="3"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="C576" s="5"/>
+      <c r="C576" s="3"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="C577" s="5"/>
+      <c r="C577" s="3"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="C578" s="5"/>
+      <c r="C578" s="3"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="C579" s="5"/>
+      <c r="C579" s="3"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="C580" s="5"/>
+      <c r="C580" s="3"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="C581" s="5"/>
+      <c r="C581" s="3"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="C582" s="5"/>
+      <c r="C582" s="3"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="C583" s="5"/>
+      <c r="C583" s="3"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="C584" s="5"/>
+      <c r="C584" s="3"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="C585" s="5"/>
+      <c r="C585" s="3"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="C586" s="5"/>
+      <c r="C586" s="3"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="C587" s="5"/>
+      <c r="C587" s="3"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="C588" s="5"/>
+      <c r="C588" s="3"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="C589" s="5"/>
+      <c r="C589" s="3"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="C590" s="5"/>
+      <c r="C590" s="3"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="C591" s="5"/>
+      <c r="C591" s="3"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="C592" s="5"/>
+      <c r="C592" s="3"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="C593" s="5"/>
+      <c r="C593" s="3"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="C594" s="5"/>
+      <c r="C594" s="3"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="C595" s="5"/>
+      <c r="C595" s="3"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="C596" s="5"/>
+      <c r="C596" s="3"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="C597" s="5"/>
+      <c r="C597" s="3"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="C598" s="5"/>
+      <c r="C598" s="3"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="C599" s="5"/>
+      <c r="C599" s="3"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="C600" s="5"/>
+      <c r="C600" s="3"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="C601" s="5"/>
+      <c r="C601" s="3"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="C602" s="5"/>
+      <c r="C602" s="3"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="C603" s="5"/>
+      <c r="C603" s="3"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="C604" s="5"/>
+      <c r="C604" s="3"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="C605" s="5"/>
+      <c r="C605" s="3"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="C606" s="5"/>
+      <c r="C606" s="3"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="C607" s="5"/>
+      <c r="C607" s="3"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="C608" s="5"/>
+      <c r="C608" s="3"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="C609" s="5"/>
+      <c r="C609" s="3"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="C610" s="5"/>
+      <c r="C610" s="3"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="C611" s="5"/>
+      <c r="C611" s="3"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="C612" s="5"/>
+      <c r="C612" s="3"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="C613" s="5"/>
+      <c r="C613" s="3"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="C614" s="5"/>
+      <c r="C614" s="3"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="C615" s="5"/>
+      <c r="C615" s="3"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="C616" s="5"/>
+      <c r="C616" s="3"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="C617" s="5"/>
+      <c r="C617" s="3"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="C618" s="5"/>
+      <c r="C618" s="3"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="C619" s="5"/>
+      <c r="C619" s="3"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="C620" s="5"/>
+      <c r="C620" s="3"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="C621" s="5"/>
+      <c r="C621" s="3"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="C622" s="5"/>
+      <c r="C622" s="3"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="C623" s="5"/>
+      <c r="C623" s="3"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="C624" s="5"/>
+      <c r="C624" s="3"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="C625" s="5"/>
+      <c r="C625" s="3"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="C626" s="5"/>
+      <c r="C626" s="3"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="C627" s="5"/>
+      <c r="C627" s="3"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="C628" s="5"/>
+      <c r="C628" s="3"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="C629" s="5"/>
+      <c r="C629" s="3"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="C630" s="5"/>
+      <c r="C630" s="3"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="C631" s="5"/>
+      <c r="C631" s="3"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="C632" s="5"/>
+      <c r="C632" s="3"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="C633" s="5"/>
+      <c r="C633" s="3"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="C634" s="5"/>
+      <c r="C634" s="3"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="C635" s="5"/>
+      <c r="C635" s="3"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="C636" s="5"/>
+      <c r="C636" s="3"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="C637" s="5"/>
+      <c r="C637" s="3"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="C638" s="5"/>
+      <c r="C638" s="3"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="C639" s="5"/>
+      <c r="C639" s="3"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="C640" s="5"/>
+      <c r="C640" s="3"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="C641" s="5"/>
+      <c r="C641" s="3"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="C642" s="5"/>
+      <c r="C642" s="3"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="C643" s="5"/>
+      <c r="C643" s="3"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="C644" s="5"/>
+      <c r="C644" s="3"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="C645" s="5"/>
+      <c r="C645" s="3"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="C646" s="5"/>
+      <c r="C646" s="3"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="C647" s="5"/>
+      <c r="C647" s="3"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="C648" s="5"/>
+      <c r="C648" s="3"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="C649" s="5"/>
+      <c r="C649" s="3"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="C650" s="5"/>
+      <c r="C650" s="3"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="C651" s="5"/>
+      <c r="C651" s="3"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="C652" s="5"/>
+      <c r="C652" s="3"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="C653" s="5"/>
+      <c r="C653" s="3"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="C654" s="5"/>
+      <c r="C654" s="3"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="C655" s="5"/>
+      <c r="C655" s="3"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="C656" s="5"/>
+      <c r="C656" s="3"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="C657" s="5"/>
+      <c r="C657" s="3"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="C658" s="5"/>
+      <c r="C658" s="3"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="C659" s="5"/>
+      <c r="C659" s="3"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="C660" s="5"/>
+      <c r="C660" s="3"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="C661" s="5"/>
+      <c r="C661" s="3"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="C662" s="5"/>
+      <c r="C662" s="3"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="C663" s="5"/>
+      <c r="C663" s="3"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="C664" s="5"/>
+      <c r="C664" s="3"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="C665" s="5"/>
+      <c r="C665" s="3"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="C666" s="5"/>
+      <c r="C666" s="3"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="C667" s="5"/>
+      <c r="C667" s="3"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="C668" s="5"/>
+      <c r="C668" s="3"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="C669" s="5"/>
+      <c r="C669" s="3"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="C670" s="5"/>
+      <c r="C670" s="3"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="C671" s="5"/>
+      <c r="C671" s="3"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="C672" s="5"/>
+      <c r="C672" s="3"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="C673" s="5"/>
+      <c r="C673" s="3"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="C674" s="5"/>
+      <c r="C674" s="3"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="C675" s="5"/>
+      <c r="C675" s="3"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="C676" s="5"/>
+      <c r="C676" s="3"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="C677" s="5"/>
+      <c r="C677" s="3"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="C678" s="5"/>
+      <c r="C678" s="3"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="C679" s="5"/>
+      <c r="C679" s="3"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="C680" s="5"/>
+      <c r="C680" s="3"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="C681" s="5"/>
+      <c r="C681" s="3"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="C682" s="5"/>
+      <c r="C682" s="3"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="C683" s="5"/>
+      <c r="C683" s="3"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="C684" s="5"/>
+      <c r="C684" s="3"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="C685" s="5"/>
+      <c r="C685" s="3"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="C686" s="5"/>
+      <c r="C686" s="3"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="C687" s="5"/>
+      <c r="C687" s="3"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="C688" s="5"/>
+      <c r="C688" s="3"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="C689" s="5"/>
+      <c r="C689" s="3"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="C690" s="5"/>
+      <c r="C690" s="3"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="C691" s="5"/>
+      <c r="C691" s="3"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="C692" s="5"/>
+      <c r="C692" s="3"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="C693" s="5"/>
+      <c r="C693" s="3"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="C694" s="5"/>
+      <c r="C694" s="3"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="C695" s="5"/>
+      <c r="C695" s="3"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="C696" s="5"/>
+      <c r="C696" s="3"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="C697" s="5"/>
+      <c r="C697" s="3"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="C698" s="5"/>
+      <c r="C698" s="3"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="C699" s="5"/>
+      <c r="C699" s="3"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="C700" s="5"/>
+      <c r="C700" s="3"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="C701" s="5"/>
+      <c r="C701" s="3"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="C702" s="5"/>
+      <c r="C702" s="3"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="C703" s="5"/>
+      <c r="C703" s="3"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="C704" s="5"/>
+      <c r="C704" s="3"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="C705" s="5"/>
+      <c r="C705" s="3"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="C706" s="5"/>
+      <c r="C706" s="3"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="C707" s="5"/>
+      <c r="C707" s="3"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="C708" s="5"/>
+      <c r="C708" s="3"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="C709" s="5"/>
+      <c r="C709" s="3"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="C710" s="5"/>
+      <c r="C710" s="3"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="C711" s="5"/>
+      <c r="C711" s="3"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="C712" s="5"/>
+      <c r="C712" s="3"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="C713" s="5"/>
+      <c r="C713" s="3"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="C714" s="5"/>
+      <c r="C714" s="3"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="C715" s="5"/>
+      <c r="C715" s="3"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="C716" s="5"/>
+      <c r="C716" s="3"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="C717" s="5"/>
+      <c r="C717" s="3"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="C718" s="5"/>
+      <c r="C718" s="3"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="C719" s="5"/>
+      <c r="C719" s="3"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="C720" s="5"/>
+      <c r="C720" s="3"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="C721" s="5"/>
+      <c r="C721" s="3"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="C722" s="5"/>
+      <c r="C722" s="3"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="C723" s="5"/>
+      <c r="C723" s="3"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="C724" s="5"/>
+      <c r="C724" s="3"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="C725" s="5"/>
+      <c r="C725" s="3"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="C726" s="5"/>
+      <c r="C726" s="3"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="C727" s="5"/>
+      <c r="C727" s="3"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="C728" s="5"/>
+      <c r="C728" s="3"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="C729" s="5"/>
+      <c r="C729" s="3"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="C730" s="5"/>
+      <c r="C730" s="3"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="C731" s="5"/>
+      <c r="C731" s="3"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="C732" s="5"/>
+      <c r="C732" s="3"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="C733" s="5"/>
+      <c r="C733" s="3"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="C734" s="5"/>
+      <c r="C734" s="3"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="C735" s="5"/>
+      <c r="C735" s="3"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="C736" s="5"/>
+      <c r="C736" s="3"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="C737" s="5"/>
+      <c r="C737" s="3"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="C738" s="5"/>
+      <c r="C738" s="3"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="C739" s="5"/>
+      <c r="C739" s="3"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="C740" s="5"/>
+      <c r="C740" s="3"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="C741" s="5"/>
+      <c r="C741" s="3"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="C742" s="5"/>
+      <c r="C742" s="3"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="C743" s="5"/>
+      <c r="C743" s="3"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="C744" s="5"/>
+      <c r="C744" s="3"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="C745" s="5"/>
+      <c r="C745" s="3"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="C746" s="5"/>
+      <c r="C746" s="3"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="C747" s="5"/>
+      <c r="C747" s="3"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="C748" s="5"/>
+      <c r="C748" s="3"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="C749" s="5"/>
+      <c r="C749" s="3"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="C750" s="5"/>
+      <c r="C750" s="3"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="C751" s="5"/>
+      <c r="C751" s="3"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="C752" s="5"/>
+      <c r="C752" s="3"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="C753" s="5"/>
+      <c r="C753" s="3"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="C754" s="5"/>
+      <c r="C754" s="3"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="C755" s="5"/>
+      <c r="C755" s="3"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="C756" s="5"/>
+      <c r="C756" s="3"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="C757" s="5"/>
+      <c r="C757" s="3"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="C758" s="5"/>
+      <c r="C758" s="3"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="C759" s="5"/>
+      <c r="C759" s="3"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="C760" s="5"/>
+      <c r="C760" s="3"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="C761" s="5"/>
+      <c r="C761" s="3"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="C762" s="5"/>
+      <c r="C762" s="3"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="C763" s="5"/>
+      <c r="C763" s="3"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="C764" s="5"/>
+      <c r="C764" s="3"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="C765" s="5"/>
+      <c r="C765" s="3"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="C766" s="5"/>
+      <c r="C766" s="3"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="C767" s="5"/>
+      <c r="C767" s="3"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="C768" s="5"/>
+      <c r="C768" s="3"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="C769" s="5"/>
+      <c r="C769" s="3"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="C770" s="5"/>
+      <c r="C770" s="3"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="C771" s="5"/>
+      <c r="C771" s="3"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="C772" s="5"/>
+      <c r="C772" s="3"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="C773" s="5"/>
+      <c r="C773" s="3"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="C774" s="5"/>
+      <c r="C774" s="3"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="C775" s="5"/>
+      <c r="C775" s="3"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="C776" s="5"/>
+      <c r="C776" s="3"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="C777" s="5"/>
+      <c r="C777" s="3"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="C778" s="5"/>
+      <c r="C778" s="3"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="C779" s="5"/>
+      <c r="C779" s="3"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="C780" s="5"/>
+      <c r="C780" s="3"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="C781" s="5"/>
+      <c r="C781" s="3"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="C782" s="5"/>
+      <c r="C782" s="3"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="C783" s="5"/>
+      <c r="C783" s="3"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="C784" s="5"/>
+      <c r="C784" s="3"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="C785" s="5"/>
+      <c r="C785" s="3"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="C786" s="5"/>
+      <c r="C786" s="3"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="C787" s="5"/>
+      <c r="C787" s="3"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="C788" s="5"/>
+      <c r="C788" s="3"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="C789" s="5"/>
+      <c r="C789" s="3"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="C790" s="5"/>
+      <c r="C790" s="3"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="C791" s="5"/>
+      <c r="C791" s="3"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="C792" s="5"/>
+      <c r="C792" s="3"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="C793" s="5"/>
+      <c r="C793" s="3"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="C794" s="5"/>
+      <c r="C794" s="3"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="C795" s="5"/>
+      <c r="C795" s="3"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="C796" s="5"/>
+      <c r="C796" s="3"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="C797" s="5"/>
+      <c r="C797" s="3"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="C798" s="5"/>
+      <c r="C798" s="3"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="C799" s="5"/>
+      <c r="C799" s="3"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="C800" s="5"/>
+      <c r="C800" s="3"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="C801" s="5"/>
+      <c r="C801" s="3"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="C802" s="5"/>
+      <c r="C802" s="3"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="C803" s="5"/>
+      <c r="C803" s="3"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="C804" s="5"/>
+      <c r="C804" s="3"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="C805" s="5"/>
+      <c r="C805" s="3"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="C806" s="5"/>
+      <c r="C806" s="3"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="C807" s="5"/>
+      <c r="C807" s="3"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="C808" s="5"/>
+      <c r="C808" s="3"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="C809" s="5"/>
+      <c r="C809" s="3"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="C810" s="5"/>
+      <c r="C810" s="3"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="C811" s="5"/>
+      <c r="C811" s="3"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="C812" s="5"/>
+      <c r="C812" s="3"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="C813" s="5"/>
+      <c r="C813" s="3"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="C814" s="5"/>
+      <c r="C814" s="3"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="C815" s="5"/>
+      <c r="C815" s="3"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="C816" s="5"/>
+      <c r="C816" s="3"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="C817" s="5"/>
+      <c r="C817" s="3"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="C818" s="5"/>
+      <c r="C818" s="3"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="C819" s="5"/>
+      <c r="C819" s="3"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="C820" s="5"/>
+      <c r="C820" s="3"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="C821" s="5"/>
+      <c r="C821" s="3"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="C822" s="5"/>
+      <c r="C822" s="3"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="C823" s="5"/>
+      <c r="C823" s="3"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="C824" s="5"/>
+      <c r="C824" s="3"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="C825" s="5"/>
+      <c r="C825" s="3"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="C826" s="5"/>
+      <c r="C826" s="3"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="C827" s="5"/>
+      <c r="C827" s="3"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="C828" s="5"/>
+      <c r="C828" s="3"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="C829" s="5"/>
+      <c r="C829" s="3"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="C830" s="5"/>
+      <c r="C830" s="3"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="C831" s="5"/>
+      <c r="C831" s="3"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="C832" s="5"/>
+      <c r="C832" s="3"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="C833" s="5"/>
+      <c r="C833" s="3"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="C834" s="5"/>
+      <c r="C834" s="3"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="C835" s="5"/>
+      <c r="C835" s="3"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="C836" s="5"/>
+      <c r="C836" s="3"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="C837" s="5"/>
+      <c r="C837" s="3"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="C838" s="5"/>
+      <c r="C838" s="3"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="C839" s="5"/>
+      <c r="C839" s="3"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="C840" s="5"/>
+      <c r="C840" s="3"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="C841" s="5"/>
+      <c r="C841" s="3"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="C842" s="5"/>
+      <c r="C842" s="3"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="C843" s="5"/>
+      <c r="C843" s="3"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="C844" s="5"/>
+      <c r="C844" s="3"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="C845" s="5"/>
+      <c r="C845" s="3"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="C846" s="5"/>
+      <c r="C846" s="3"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="C847" s="5"/>
+      <c r="C847" s="3"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="C848" s="5"/>
+      <c r="C848" s="3"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="C849" s="5"/>
+      <c r="C849" s="3"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="C850" s="5"/>
+      <c r="C850" s="3"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="C851" s="5"/>
+      <c r="C851" s="3"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="C852" s="5"/>
+      <c r="C852" s="3"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="C853" s="5"/>
+      <c r="C853" s="3"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="C854" s="5"/>
+      <c r="C854" s="3"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="C855" s="5"/>
+      <c r="C855" s="3"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="C856" s="5"/>
+      <c r="C856" s="3"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="C857" s="5"/>
+      <c r="C857" s="3"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="C858" s="5"/>
+      <c r="C858" s="3"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="C859" s="5"/>
+      <c r="C859" s="3"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="C860" s="5"/>
+      <c r="C860" s="3"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="C861" s="5"/>
+      <c r="C861" s="3"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="C862" s="5"/>
+      <c r="C862" s="3"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="C863" s="5"/>
+      <c r="C863" s="3"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="C864" s="5"/>
+      <c r="C864" s="3"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="C865" s="5"/>
+      <c r="C865" s="3"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="C866" s="5"/>
+      <c r="C866" s="3"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="C867" s="5"/>
+      <c r="C867" s="3"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="C868" s="5"/>
+      <c r="C868" s="3"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="C869" s="5"/>
+      <c r="C869" s="3"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="C870" s="5"/>
+      <c r="C870" s="3"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="C871" s="5"/>
+      <c r="C871" s="3"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="C872" s="5"/>
+      <c r="C872" s="3"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="C873" s="5"/>
+      <c r="C873" s="3"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="C874" s="5"/>
+      <c r="C874" s="3"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="C875" s="5"/>
+      <c r="C875" s="3"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="C876" s="5"/>
+      <c r="C876" s="3"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="C877" s="5"/>
+      <c r="C877" s="3"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="C878" s="5"/>
+      <c r="C878" s="3"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="C879" s="5"/>
+      <c r="C879" s="3"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="C880" s="5"/>
+      <c r="C880" s="3"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="C881" s="5"/>
+      <c r="C881" s="3"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="C882" s="5"/>
+      <c r="C882" s="3"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="C883" s="5"/>
+      <c r="C883" s="3"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="C884" s="5"/>
+      <c r="C884" s="3"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="C885" s="5"/>
+      <c r="C885" s="3"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="C886" s="5"/>
+      <c r="C886" s="3"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="C887" s="5"/>
+      <c r="C887" s="3"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="C888" s="5"/>
+      <c r="C888" s="3"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="C889" s="5"/>
+      <c r="C889" s="3"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="C890" s="5"/>
+      <c r="C890" s="3"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="C891" s="5"/>
+      <c r="C891" s="3"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="C892" s="5"/>
+      <c r="C892" s="3"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="C893" s="5"/>
+      <c r="C893" s="3"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="C894" s="5"/>
+      <c r="C894" s="3"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="C895" s="5"/>
+      <c r="C895" s="3"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="C896" s="5"/>
+      <c r="C896" s="3"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="C897" s="5"/>
+      <c r="C897" s="3"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="C898" s="5"/>
+      <c r="C898" s="3"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="C899" s="5"/>
+      <c r="C899" s="3"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="C900" s="5"/>
+      <c r="C900" s="3"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="C901" s="5"/>
+      <c r="C901" s="3"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="C902" s="5"/>
+      <c r="C902" s="3"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="C903" s="5"/>
+      <c r="C903" s="3"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="C904" s="5"/>
+      <c r="C904" s="3"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="C905" s="5"/>
+      <c r="C905" s="3"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="C906" s="5"/>
+      <c r="C906" s="3"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="C907" s="5"/>
+      <c r="C907" s="3"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="C908" s="5"/>
+      <c r="C908" s="3"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="C909" s="5"/>
+      <c r="C909" s="3"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="C910" s="5"/>
+      <c r="C910" s="3"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="C911" s="5"/>
+      <c r="C911" s="3"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="C912" s="5"/>
+      <c r="C912" s="3"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="C913" s="5"/>
+      <c r="C913" s="3"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="C914" s="5"/>
+      <c r="C914" s="3"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="C915" s="5"/>
+      <c r="C915" s="3"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="C916" s="5"/>
+      <c r="C916" s="3"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="C917" s="5"/>
+      <c r="C917" s="3"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="C918" s="5"/>
+      <c r="C918" s="3"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="C919" s="5"/>
+      <c r="C919" s="3"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="C920" s="5"/>
+      <c r="C920" s="3"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="C921" s="5"/>
+      <c r="C921" s="3"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="C922" s="5"/>
+      <c r="C922" s="3"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="C923" s="5"/>
+      <c r="C923" s="3"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="C924" s="5"/>
+      <c r="C924" s="3"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="C925" s="5"/>
+      <c r="C925" s="3"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="C926" s="5"/>
+      <c r="C926" s="3"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="C927" s="5"/>
+      <c r="C927" s="3"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="C928" s="5"/>
+      <c r="C928" s="3"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="C929" s="5"/>
+      <c r="C929" s="3"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="C930" s="5"/>
+      <c r="C930" s="3"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="C931" s="5"/>
+      <c r="C931" s="3"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="C932" s="5"/>
+      <c r="C932" s="3"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="C933" s="5"/>
+      <c r="C933" s="3"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="C934" s="5"/>
+      <c r="C934" s="3"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="C935" s="5"/>
+      <c r="C935" s="3"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="C936" s="5"/>
+      <c r="C936" s="3"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="C937" s="5"/>
+      <c r="C937" s="3"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="C938" s="5"/>
+      <c r="C938" s="3"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="C939" s="5"/>
+      <c r="C939" s="3"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="C940" s="5"/>
+      <c r="C940" s="3"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="C941" s="5"/>
+      <c r="C941" s="3"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="C942" s="5"/>
+      <c r="C942" s="3"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="C943" s="5"/>
+      <c r="C943" s="3"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="C944" s="5"/>
+      <c r="C944" s="3"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="C945" s="5"/>
+      <c r="C945" s="3"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="C946" s="5"/>
+      <c r="C946" s="3"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="C947" s="5"/>
+      <c r="C947" s="3"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="C948" s="5"/>
+      <c r="C948" s="3"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="C949" s="5"/>
+      <c r="C949" s="3"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="C950" s="5"/>
+      <c r="C950" s="3"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="C951" s="5"/>
+      <c r="C951" s="3"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="C952" s="5"/>
+      <c r="C952" s="3"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="C953" s="5"/>
+      <c r="C953" s="3"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="C954" s="5"/>
+      <c r="C954" s="3"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="C955" s="5"/>
+      <c r="C955" s="3"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="C956" s="5"/>
+      <c r="C956" s="3"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="C957" s="5"/>
+      <c r="C957" s="3"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="C958" s="5"/>
+      <c r="C958" s="3"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="C959" s="5"/>
+      <c r="C959" s="3"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="C960" s="5"/>
+      <c r="C960" s="3"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="C961" s="5"/>
+      <c r="C961" s="3"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="C962" s="5"/>
+      <c r="C962" s="3"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="C963" s="5"/>
+      <c r="C963" s="3"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="C964" s="5"/>
+      <c r="C964" s="3"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="C965" s="5"/>
+      <c r="C965" s="3"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="C966" s="5"/>
+      <c r="C966" s="3"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="C967" s="5"/>
+      <c r="C967" s="3"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="C968" s="5"/>
+      <c r="C968" s="3"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="C969" s="5"/>
+      <c r="C969" s="3"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="C970" s="5"/>
+      <c r="C970" s="3"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="C971" s="5"/>
+      <c r="C971" s="3"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="C972" s="5"/>
+      <c r="C972" s="3"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="C973" s="5"/>
+      <c r="C973" s="3"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="C974" s="5"/>
+      <c r="C974" s="3"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="C975" s="5"/>
+      <c r="C975" s="3"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="C976" s="5"/>
+      <c r="C976" s="3"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="C977" s="5"/>
+      <c r="C977" s="3"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="C978" s="5"/>
+      <c r="C978" s="3"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="C979" s="5"/>
+      <c r="C979" s="3"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="C980" s="5"/>
+      <c r="C980" s="3"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="C981" s="5"/>
+      <c r="C981" s="3"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="C982" s="5"/>
+      <c r="C982" s="3"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="C983" s="5"/>
+      <c r="C983" s="3"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="C984" s="5"/>
+      <c r="C984" s="3"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="C985" s="5"/>
+      <c r="C985" s="3"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="C986" s="5"/>
+      <c r="C986" s="3"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="C987" s="5"/>
+      <c r="C987" s="3"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="C988" s="5"/>
+      <c r="C988" s="3"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="C989" s="5"/>
+      <c r="C989" s="3"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="C990" s="5"/>
+      <c r="C990" s="3"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="C991" s="5"/>
+      <c r="C991" s="3"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="C992" s="5"/>
+      <c r="C992" s="3"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="C993" s="5"/>
+      <c r="C993" s="3"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="C994" s="5"/>
+      <c r="C994" s="3"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
-      <c r="C995" s="5"/>
+      <c r="C995" s="3"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
-      <c r="C996" s="5"/>
+      <c r="C996" s="3"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
-      <c r="C997" s="5"/>
+      <c r="C997" s="3"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
-      <c r="C998" s="5"/>
+      <c r="C998" s="3"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
-      <c r="C999" s="5"/>
+      <c r="C999" s="3"/>
     </row>
     <row r="1000" ht="15.75" customHeight="1">
-      <c r="C1000" s="5"/>
+      <c r="C1000" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1000">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1000">
-      <formula1>'Hoja 2'!$A$2:$A$9</formula1>
+      <formula1>'Hoja 2'!$A$2:$A$13</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -3639,19 +3666,35 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
quoter 0 price bug fix2
</commit_message>
<xml_diff>
--- a/files/onboarding/Agroassist_Plantilla_Onboarding.xlsx
+++ b/files/onboarding/Agroassist_Plantilla_Onboarding.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>CSG</t>
+  </si>
   <si>
     <t>Nombre Cuartel</t>
   </si>
@@ -63,6 +66,12 @@
   </si>
   <si>
     <t>Castaños</t>
+  </si>
+  <si>
+    <t>Duraznos</t>
+  </si>
+  <si>
+    <t>Kiwis</t>
   </si>
 </sst>
 </file>
@@ -120,14 +129,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -362,9 +375,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="12.63"/>
-    <col customWidth="1" min="3" max="3" width="16.88"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
+    <col customWidth="1" min="1" max="3" width="12.63"/>
+    <col customWidth="1" min="4" max="4" width="16.88"/>
+    <col customWidth="1" min="5" max="7" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -374,3242 +387,3250 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="4"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="4"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="4"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="4"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="4"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="4"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="4"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="B39" s="4"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="B40" s="4"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="4"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="4"/>
-      <c r="C42" s="3"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="B43" s="4"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="4"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="4"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="4"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="4"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="4"/>
-      <c r="C48" s="3"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="4"/>
-      <c r="C49" s="3"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="4"/>
-      <c r="C50" s="3"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="4"/>
-      <c r="C51" s="3"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="4"/>
-      <c r="C52" s="3"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="4"/>
-      <c r="C53" s="3"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="4"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="4"/>
-      <c r="C54" s="3"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="4"/>
-      <c r="C55" s="3"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="4"/>
-      <c r="C56" s="3"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="4"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="4"/>
-      <c r="C57" s="3"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="B58" s="4"/>
-      <c r="C58" s="3"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="4"/>
-      <c r="C59" s="3"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="B60" s="4"/>
-      <c r="C60" s="3"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="4"/>
-      <c r="C61" s="3"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="4"/>
-      <c r="C62" s="3"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="4"/>
-      <c r="C63" s="3"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="4"/>
-      <c r="C64" s="3"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="4"/>
-      <c r="C65" s="3"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="4"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="4"/>
-      <c r="C66" s="3"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="4"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="4"/>
-      <c r="C67" s="3"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="4"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="4"/>
-      <c r="C68" s="3"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="4"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="B69" s="4"/>
-      <c r="C69" s="3"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="B70" s="4"/>
-      <c r="C70" s="3"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="4"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="4"/>
-      <c r="C71" s="3"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="4"/>
-      <c r="C72" s="3"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="4"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="4"/>
-      <c r="C73" s="3"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="4"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="4"/>
-      <c r="C74" s="3"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="B75" s="4"/>
-      <c r="C75" s="3"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="4"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="B76" s="4"/>
-      <c r="C76" s="3"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="4"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="B77" s="4"/>
-      <c r="C77" s="3"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="4"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="B78" s="4"/>
-      <c r="C78" s="3"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="4"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="B79" s="4"/>
-      <c r="C79" s="3"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="4"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="B80" s="4"/>
-      <c r="C80" s="3"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="4"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="B81" s="4"/>
-      <c r="C81" s="3"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="4"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="B82" s="4"/>
-      <c r="C82" s="3"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="4"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="B83" s="4"/>
-      <c r="C83" s="3"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="B84" s="4"/>
-      <c r="C84" s="3"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="4"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="B85" s="4"/>
-      <c r="C85" s="3"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="4"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="B86" s="4"/>
-      <c r="C86" s="3"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="4"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="B87" s="4"/>
-      <c r="C87" s="3"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="4"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="B88" s="4"/>
-      <c r="C88" s="3"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="4"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="B89" s="4"/>
-      <c r="C89" s="3"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="4"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="B90" s="4"/>
-      <c r="C90" s="3"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="4"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="B91" s="4"/>
-      <c r="C91" s="3"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="4"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="B92" s="4"/>
-      <c r="C92" s="3"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="4"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="B93" s="4"/>
-      <c r="C93" s="3"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="4"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="B94" s="4"/>
-      <c r="C94" s="3"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="4"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="B95" s="4"/>
-      <c r="C95" s="3"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="4"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="B96" s="4"/>
-      <c r="C96" s="3"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="4"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="B97" s="4"/>
-      <c r="C97" s="3"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="4"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="B98" s="4"/>
-      <c r="C98" s="3"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="4"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="B99" s="4"/>
-      <c r="C99" s="3"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="4"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="B100" s="4"/>
-      <c r="C100" s="3"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="4"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="B101" s="4"/>
-      <c r="C101" s="3"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="4"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="B102" s="4"/>
-      <c r="C102" s="3"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="4"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="B103" s="4"/>
-      <c r="C103" s="3"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="4"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="B104" s="4"/>
-      <c r="C104" s="3"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="4"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="B105" s="4"/>
-      <c r="C105" s="3"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="4"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="B106" s="4"/>
-      <c r="C106" s="3"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="4"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="B107" s="4"/>
-      <c r="C107" s="3"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="4"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="B108" s="4"/>
-      <c r="C108" s="3"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="4"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="B109" s="4"/>
-      <c r="C109" s="3"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="4"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="B110" s="4"/>
-      <c r="C110" s="3"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="4"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="B111" s="4"/>
-      <c r="C111" s="3"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="4"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="B112" s="4"/>
-      <c r="C112" s="3"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="4"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="B113" s="4"/>
-      <c r="C113" s="3"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="4"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="B114" s="4"/>
-      <c r="C114" s="3"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="4"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="B115" s="4"/>
-      <c r="C115" s="3"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="4"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="B116" s="4"/>
-      <c r="C116" s="3"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="4"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="B117" s="4"/>
-      <c r="C117" s="3"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="4"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="B118" s="4"/>
-      <c r="C118" s="3"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="4"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="B119" s="4"/>
-      <c r="C119" s="3"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="4"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="B120" s="4"/>
-      <c r="C120" s="3"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="4"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="B121" s="4"/>
-      <c r="C121" s="3"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="4"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="B122" s="4"/>
-      <c r="C122" s="3"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="4"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="B123" s="4"/>
-      <c r="C123" s="3"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="4"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="B124" s="4"/>
-      <c r="C124" s="3"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="4"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="B125" s="4"/>
-      <c r="C125" s="3"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="4"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="B126" s="4"/>
-      <c r="C126" s="3"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="4"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="B127" s="4"/>
-      <c r="C127" s="3"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="4"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="B128" s="4"/>
-      <c r="C128" s="3"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="4"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="B129" s="4"/>
-      <c r="C129" s="3"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="4"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="B130" s="4"/>
-      <c r="C130" s="3"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="4"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="B131" s="4"/>
-      <c r="C131" s="3"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="4"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="B132" s="4"/>
-      <c r="C132" s="3"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="4"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="B133" s="4"/>
-      <c r="C133" s="3"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="4"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="B134" s="4"/>
-      <c r="C134" s="3"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="4"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="B135" s="4"/>
-      <c r="C135" s="3"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="4"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="B136" s="4"/>
-      <c r="C136" s="3"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="4"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="B137" s="4"/>
-      <c r="C137" s="3"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="4"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="B138" s="4"/>
-      <c r="C138" s="3"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="4"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="B139" s="4"/>
-      <c r="C139" s="3"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="4"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="B140" s="4"/>
-      <c r="C140" s="3"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="4"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="B141" s="4"/>
-      <c r="C141" s="3"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="4"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="B142" s="4"/>
-      <c r="C142" s="3"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="4"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="B143" s="4"/>
-      <c r="C143" s="3"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="4"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="B144" s="4"/>
-      <c r="C144" s="3"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="4"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="B145" s="4"/>
-      <c r="C145" s="3"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="4"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="B146" s="4"/>
-      <c r="C146" s="3"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="4"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="B147" s="4"/>
-      <c r="C147" s="3"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="4"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="B148" s="4"/>
-      <c r="C148" s="3"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="4"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="B149" s="4"/>
-      <c r="C149" s="3"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="4"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="B150" s="4"/>
-      <c r="C150" s="3"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="4"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="B151" s="4"/>
-      <c r="C151" s="3"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="4"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="B152" s="4"/>
-      <c r="C152" s="3"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="4"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="B153" s="4"/>
-      <c r="C153" s="3"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="4"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="B154" s="4"/>
-      <c r="C154" s="3"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="4"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="B155" s="4"/>
-      <c r="C155" s="3"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="4"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="B156" s="4"/>
-      <c r="C156" s="3"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="4"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="B157" s="4"/>
-      <c r="C157" s="3"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="4"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="B158" s="4"/>
-      <c r="C158" s="3"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="4"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="B159" s="4"/>
-      <c r="C159" s="3"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="4"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="B160" s="4"/>
-      <c r="C160" s="3"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="4"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="B161" s="4"/>
-      <c r="C161" s="3"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="4"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="B162" s="4"/>
-      <c r="C162" s="3"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="4"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="B163" s="4"/>
-      <c r="C163" s="3"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="4"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="B164" s="4"/>
-      <c r="C164" s="3"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="4"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="B165" s="4"/>
-      <c r="C165" s="3"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="4"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="B166" s="4"/>
-      <c r="C166" s="3"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="4"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="B167" s="4"/>
-      <c r="C167" s="3"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="4"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="B168" s="4"/>
-      <c r="C168" s="3"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="4"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="B169" s="4"/>
-      <c r="C169" s="3"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="4"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="B170" s="4"/>
-      <c r="C170" s="3"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="4"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="B171" s="4"/>
-      <c r="C171" s="3"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="4"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="B172" s="4"/>
-      <c r="C172" s="3"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="4"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="B173" s="4"/>
-      <c r="C173" s="3"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="4"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="B174" s="4"/>
-      <c r="C174" s="3"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="4"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="B175" s="4"/>
-      <c r="C175" s="3"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="4"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="B176" s="4"/>
-      <c r="C176" s="3"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="4"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="B177" s="4"/>
-      <c r="C177" s="3"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="4"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="B178" s="4"/>
-      <c r="C178" s="3"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="4"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="B179" s="4"/>
-      <c r="C179" s="3"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="4"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="B180" s="4"/>
-      <c r="C180" s="3"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="4"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="B181" s="4"/>
-      <c r="C181" s="3"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="4"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="B182" s="4"/>
-      <c r="C182" s="3"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="4"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="B183" s="4"/>
-      <c r="C183" s="3"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="4"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="B184" s="4"/>
-      <c r="C184" s="3"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="4"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="B185" s="4"/>
-      <c r="C185" s="3"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="4"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="B186" s="4"/>
-      <c r="C186" s="3"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="4"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="B187" s="4"/>
-      <c r="C187" s="3"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="4"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="4"/>
-      <c r="C188" s="3"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="4"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="B189" s="4"/>
-      <c r="C189" s="3"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="4"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="B190" s="4"/>
-      <c r="C190" s="3"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="4"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="B191" s="4"/>
-      <c r="C191" s="3"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="4"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="B192" s="4"/>
-      <c r="C192" s="3"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="4"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="B193" s="4"/>
-      <c r="C193" s="3"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="4"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="B194" s="4"/>
-      <c r="C194" s="3"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="4"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="B195" s="4"/>
-      <c r="C195" s="3"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="4"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="B196" s="4"/>
-      <c r="C196" s="3"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="4"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="B197" s="4"/>
-      <c r="C197" s="3"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="4"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="B198" s="4"/>
-      <c r="C198" s="3"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="4"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="B199" s="4"/>
-      <c r="C199" s="3"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="4"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="B200" s="4"/>
-      <c r="C200" s="3"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="4"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="B201" s="4"/>
-      <c r="C201" s="3"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="4"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="B202" s="4"/>
-      <c r="C202" s="3"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="4"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="B203" s="4"/>
-      <c r="C203" s="3"/>
+      <c r="C203" s="5"/>
+      <c r="D203" s="4"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="B204" s="4"/>
-      <c r="C204" s="3"/>
+      <c r="C204" s="5"/>
+      <c r="D204" s="4"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="B205" s="4"/>
-      <c r="C205" s="3"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="4"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="B206" s="4"/>
-      <c r="C206" s="3"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="4"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="B207" s="4"/>
-      <c r="C207" s="3"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="4"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="B208" s="4"/>
-      <c r="C208" s="3"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="4"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="B209" s="4"/>
-      <c r="C209" s="3"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="4"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="B210" s="4"/>
-      <c r="C210" s="3"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="4"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="B211" s="4"/>
-      <c r="C211" s="3"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="4"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="B212" s="4"/>
-      <c r="C212" s="3"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="4"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="B213" s="4"/>
-      <c r="C213" s="3"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="4"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="B214" s="4"/>
-      <c r="C214" s="3"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="4"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="B215" s="4"/>
-      <c r="C215" s="3"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="4"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="B216" s="4"/>
-      <c r="C216" s="3"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="4"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="B217" s="4"/>
-      <c r="C217" s="3"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="4"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="B218" s="4"/>
-      <c r="C218" s="3"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="4"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="B219" s="4"/>
-      <c r="C219" s="3"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="4"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="B220" s="4"/>
-      <c r="C220" s="3"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="4"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="C221" s="3"/>
+      <c r="D221" s="4"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="C222" s="3"/>
+      <c r="D222" s="4"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="C223" s="3"/>
+      <c r="D223" s="4"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="C224" s="3"/>
+      <c r="D224" s="4"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="C225" s="3"/>
+      <c r="D225" s="4"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="C226" s="3"/>
+      <c r="D226" s="4"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="C227" s="3"/>
+      <c r="D227" s="4"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="C228" s="3"/>
+      <c r="D228" s="4"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="C229" s="3"/>
+      <c r="D229" s="4"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="C230" s="3"/>
+      <c r="D230" s="4"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="C231" s="3"/>
+      <c r="D231" s="4"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="C232" s="3"/>
+      <c r="D232" s="4"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="C233" s="3"/>
+      <c r="D233" s="4"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="C234" s="3"/>
+      <c r="D234" s="4"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="C235" s="3"/>
+      <c r="D235" s="4"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="C236" s="3"/>
+      <c r="D236" s="4"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="C237" s="3"/>
+      <c r="D237" s="4"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="C238" s="3"/>
+      <c r="D238" s="4"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="C239" s="3"/>
+      <c r="D239" s="4"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="C240" s="3"/>
+      <c r="D240" s="4"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="C241" s="3"/>
+      <c r="D241" s="4"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="C242" s="3"/>
+      <c r="D242" s="4"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="C243" s="3"/>
+      <c r="D243" s="4"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="C244" s="3"/>
+      <c r="D244" s="4"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="C245" s="3"/>
+      <c r="D245" s="4"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="C246" s="3"/>
+      <c r="D246" s="4"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="C247" s="3"/>
+      <c r="D247" s="4"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="C248" s="3"/>
+      <c r="D248" s="4"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="C249" s="3"/>
+      <c r="D249" s="4"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="C250" s="3"/>
+      <c r="D250" s="4"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="C251" s="3"/>
+      <c r="D251" s="4"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="C252" s="3"/>
+      <c r="D252" s="4"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="C253" s="3"/>
+      <c r="D253" s="4"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="C254" s="3"/>
+      <c r="D254" s="4"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="C255" s="3"/>
+      <c r="D255" s="4"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="C256" s="3"/>
+      <c r="D256" s="4"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="C257" s="3"/>
+      <c r="D257" s="4"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="C258" s="3"/>
+      <c r="D258" s="4"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="C259" s="3"/>
+      <c r="D259" s="4"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="C260" s="3"/>
+      <c r="D260" s="4"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="C261" s="3"/>
+      <c r="D261" s="4"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="C262" s="3"/>
+      <c r="D262" s="4"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="C263" s="3"/>
+      <c r="D263" s="4"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="C264" s="3"/>
+      <c r="D264" s="4"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="C265" s="3"/>
+      <c r="D265" s="4"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="C266" s="3"/>
+      <c r="D266" s="4"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="C267" s="3"/>
+      <c r="D267" s="4"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="C268" s="3"/>
+      <c r="D268" s="4"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="C269" s="3"/>
+      <c r="D269" s="4"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="C270" s="3"/>
+      <c r="D270" s="4"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="C271" s="3"/>
+      <c r="D271" s="4"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="C272" s="3"/>
+      <c r="D272" s="4"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="C273" s="3"/>
+      <c r="D273" s="4"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="C274" s="3"/>
+      <c r="D274" s="4"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="C275" s="3"/>
+      <c r="D275" s="4"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="C276" s="3"/>
+      <c r="D276" s="4"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="C277" s="3"/>
+      <c r="D277" s="4"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="C278" s="3"/>
+      <c r="D278" s="4"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="C279" s="3"/>
+      <c r="D279" s="4"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="C280" s="3"/>
+      <c r="D280" s="4"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="C281" s="3"/>
+      <c r="D281" s="4"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="C282" s="3"/>
+      <c r="D282" s="4"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="C283" s="3"/>
+      <c r="D283" s="4"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="C284" s="3"/>
+      <c r="D284" s="4"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="C285" s="3"/>
+      <c r="D285" s="4"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="C286" s="3"/>
+      <c r="D286" s="4"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="C287" s="3"/>
+      <c r="D287" s="4"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="C288" s="3"/>
+      <c r="D288" s="4"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="C289" s="3"/>
+      <c r="D289" s="4"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="C290" s="3"/>
+      <c r="D290" s="4"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="C291" s="3"/>
+      <c r="D291" s="4"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="C292" s="3"/>
+      <c r="D292" s="4"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="C293" s="3"/>
+      <c r="D293" s="4"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="C294" s="3"/>
+      <c r="D294" s="4"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="C295" s="3"/>
+      <c r="D295" s="4"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="C296" s="3"/>
+      <c r="D296" s="4"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="C297" s="3"/>
+      <c r="D297" s="4"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="C298" s="3"/>
+      <c r="D298" s="4"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="C299" s="3"/>
+      <c r="D299" s="4"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="C300" s="3"/>
+      <c r="D300" s="4"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="C301" s="3"/>
+      <c r="D301" s="4"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="C302" s="3"/>
+      <c r="D302" s="4"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="C303" s="3"/>
+      <c r="D303" s="4"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="C304" s="3"/>
+      <c r="D304" s="4"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="C305" s="3"/>
+      <c r="D305" s="4"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="C306" s="3"/>
+      <c r="D306" s="4"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="C307" s="3"/>
+      <c r="D307" s="4"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="C308" s="3"/>
+      <c r="D308" s="4"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="C309" s="3"/>
+      <c r="D309" s="4"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="C310" s="3"/>
+      <c r="D310" s="4"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="C311" s="3"/>
+      <c r="D311" s="4"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="C312" s="3"/>
+      <c r="D312" s="4"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="C313" s="3"/>
+      <c r="D313" s="4"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="C314" s="3"/>
+      <c r="D314" s="4"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="C315" s="3"/>
+      <c r="D315" s="4"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="C316" s="3"/>
+      <c r="D316" s="4"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="C317" s="3"/>
+      <c r="D317" s="4"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="C318" s="3"/>
+      <c r="D318" s="4"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="C319" s="3"/>
+      <c r="D319" s="4"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="C320" s="3"/>
+      <c r="D320" s="4"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="C321" s="3"/>
+      <c r="D321" s="4"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="C322" s="3"/>
+      <c r="D322" s="4"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="C323" s="3"/>
+      <c r="D323" s="4"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="C324" s="3"/>
+      <c r="D324" s="4"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="C325" s="3"/>
+      <c r="D325" s="4"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="C326" s="3"/>
+      <c r="D326" s="4"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="C327" s="3"/>
+      <c r="D327" s="4"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="C328" s="3"/>
+      <c r="D328" s="4"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="C329" s="3"/>
+      <c r="D329" s="4"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="C330" s="3"/>
+      <c r="D330" s="4"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="C331" s="3"/>
+      <c r="D331" s="4"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="C332" s="3"/>
+      <c r="D332" s="4"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="C333" s="3"/>
+      <c r="D333" s="4"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="C334" s="3"/>
+      <c r="D334" s="4"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="C335" s="3"/>
+      <c r="D335" s="4"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="C336" s="3"/>
+      <c r="D336" s="4"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="C337" s="3"/>
+      <c r="D337" s="4"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="C338" s="3"/>
+      <c r="D338" s="4"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="C339" s="3"/>
+      <c r="D339" s="4"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="C340" s="3"/>
+      <c r="D340" s="4"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="C341" s="3"/>
+      <c r="D341" s="4"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="C342" s="3"/>
+      <c r="D342" s="4"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="C343" s="3"/>
+      <c r="D343" s="4"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="C344" s="3"/>
+      <c r="D344" s="4"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="C345" s="3"/>
+      <c r="D345" s="4"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="C346" s="3"/>
+      <c r="D346" s="4"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="C347" s="3"/>
+      <c r="D347" s="4"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="C348" s="3"/>
+      <c r="D348" s="4"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="C349" s="3"/>
+      <c r="D349" s="4"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="C350" s="3"/>
+      <c r="D350" s="4"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="C351" s="3"/>
+      <c r="D351" s="4"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="C352" s="3"/>
+      <c r="D352" s="4"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="C353" s="3"/>
+      <c r="D353" s="4"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="C354" s="3"/>
+      <c r="D354" s="4"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="C355" s="3"/>
+      <c r="D355" s="4"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="C356" s="3"/>
+      <c r="D356" s="4"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="C357" s="3"/>
+      <c r="D357" s="4"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="C358" s="3"/>
+      <c r="D358" s="4"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="C359" s="3"/>
+      <c r="D359" s="4"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="C360" s="3"/>
+      <c r="D360" s="4"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="C361" s="3"/>
+      <c r="D361" s="4"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="C362" s="3"/>
+      <c r="D362" s="4"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="C363" s="3"/>
+      <c r="D363" s="4"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="C364" s="3"/>
+      <c r="D364" s="4"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="C365" s="3"/>
+      <c r="D365" s="4"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="C366" s="3"/>
+      <c r="D366" s="4"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="C367" s="3"/>
+      <c r="D367" s="4"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="C368" s="3"/>
+      <c r="D368" s="4"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="C369" s="3"/>
+      <c r="D369" s="4"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="C370" s="3"/>
+      <c r="D370" s="4"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="C371" s="3"/>
+      <c r="D371" s="4"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="C372" s="3"/>
+      <c r="D372" s="4"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="C373" s="3"/>
+      <c r="D373" s="4"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="C374" s="3"/>
+      <c r="D374" s="4"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="C375" s="3"/>
+      <c r="D375" s="4"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="C376" s="3"/>
+      <c r="D376" s="4"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="C377" s="3"/>
+      <c r="D377" s="4"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="C378" s="3"/>
+      <c r="D378" s="4"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="C379" s="3"/>
+      <c r="D379" s="4"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="C380" s="3"/>
+      <c r="D380" s="4"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="C381" s="3"/>
+      <c r="D381" s="4"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="C382" s="3"/>
+      <c r="D382" s="4"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="C383" s="3"/>
+      <c r="D383" s="4"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="C384" s="3"/>
+      <c r="D384" s="4"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="C385" s="3"/>
+      <c r="D385" s="4"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="C386" s="3"/>
+      <c r="D386" s="4"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="C387" s="3"/>
+      <c r="D387" s="4"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="C388" s="3"/>
+      <c r="D388" s="4"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="C389" s="3"/>
+      <c r="D389" s="4"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="C390" s="3"/>
+      <c r="D390" s="4"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="C391" s="3"/>
+      <c r="D391" s="4"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="C392" s="3"/>
+      <c r="D392" s="4"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="C393" s="3"/>
+      <c r="D393" s="4"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="C394" s="3"/>
+      <c r="D394" s="4"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="C395" s="3"/>
+      <c r="D395" s="4"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="C396" s="3"/>
+      <c r="D396" s="4"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="C397" s="3"/>
+      <c r="D397" s="4"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="C398" s="3"/>
+      <c r="D398" s="4"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="C399" s="3"/>
+      <c r="D399" s="4"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="C400" s="3"/>
+      <c r="D400" s="4"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="C401" s="3"/>
+      <c r="D401" s="4"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="C402" s="3"/>
+      <c r="D402" s="4"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="C403" s="3"/>
+      <c r="D403" s="4"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="C404" s="3"/>
+      <c r="D404" s="4"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="C405" s="3"/>
+      <c r="D405" s="4"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="C406" s="3"/>
+      <c r="D406" s="4"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="C407" s="3"/>
+      <c r="D407" s="4"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="C408" s="3"/>
+      <c r="D408" s="4"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="C409" s="3"/>
+      <c r="D409" s="4"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="C410" s="3"/>
+      <c r="D410" s="4"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="C411" s="3"/>
+      <c r="D411" s="4"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="C412" s="3"/>
+      <c r="D412" s="4"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="C413" s="3"/>
+      <c r="D413" s="4"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="C414" s="3"/>
+      <c r="D414" s="4"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="C415" s="3"/>
+      <c r="D415" s="4"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="C416" s="3"/>
+      <c r="D416" s="4"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="C417" s="3"/>
+      <c r="D417" s="4"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="C418" s="3"/>
+      <c r="D418" s="4"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="C419" s="3"/>
+      <c r="D419" s="4"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="C420" s="3"/>
+      <c r="D420" s="4"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="C421" s="3"/>
+      <c r="D421" s="4"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="C422" s="3"/>
+      <c r="D422" s="4"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="C423" s="3"/>
+      <c r="D423" s="4"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="C424" s="3"/>
+      <c r="D424" s="4"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="C425" s="3"/>
+      <c r="D425" s="4"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="C426" s="3"/>
+      <c r="D426" s="4"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="C427" s="3"/>
+      <c r="D427" s="4"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="C428" s="3"/>
+      <c r="D428" s="4"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="C429" s="3"/>
+      <c r="D429" s="4"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="C430" s="3"/>
+      <c r="D430" s="4"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="C431" s="3"/>
+      <c r="D431" s="4"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="C432" s="3"/>
+      <c r="D432" s="4"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="C433" s="3"/>
+      <c r="D433" s="4"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="C434" s="3"/>
+      <c r="D434" s="4"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="C435" s="3"/>
+      <c r="D435" s="4"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="C436" s="3"/>
+      <c r="D436" s="4"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="C437" s="3"/>
+      <c r="D437" s="4"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="C438" s="3"/>
+      <c r="D438" s="4"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="C439" s="3"/>
+      <c r="D439" s="4"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="C440" s="3"/>
+      <c r="D440" s="4"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="C441" s="3"/>
+      <c r="D441" s="4"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="C442" s="3"/>
+      <c r="D442" s="4"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="C443" s="3"/>
+      <c r="D443" s="4"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="C444" s="3"/>
+      <c r="D444" s="4"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="C445" s="3"/>
+      <c r="D445" s="4"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="C446" s="3"/>
+      <c r="D446" s="4"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="C447" s="3"/>
+      <c r="D447" s="4"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="C448" s="3"/>
+      <c r="D448" s="4"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="C449" s="3"/>
+      <c r="D449" s="4"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="C450" s="3"/>
+      <c r="D450" s="4"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="C451" s="3"/>
+      <c r="D451" s="4"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="C452" s="3"/>
+      <c r="D452" s="4"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="C453" s="3"/>
+      <c r="D453" s="4"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="C454" s="3"/>
+      <c r="D454" s="4"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="C455" s="3"/>
+      <c r="D455" s="4"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="C456" s="3"/>
+      <c r="D456" s="4"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="C457" s="3"/>
+      <c r="D457" s="4"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="C458" s="3"/>
+      <c r="D458" s="4"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="C459" s="3"/>
+      <c r="D459" s="4"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="C460" s="3"/>
+      <c r="D460" s="4"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="C461" s="3"/>
+      <c r="D461" s="4"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="C462" s="3"/>
+      <c r="D462" s="4"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="C463" s="3"/>
+      <c r="D463" s="4"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="C464" s="3"/>
+      <c r="D464" s="4"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="C465" s="3"/>
+      <c r="D465" s="4"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="C466" s="3"/>
+      <c r="D466" s="4"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="C467" s="3"/>
+      <c r="D467" s="4"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="C468" s="3"/>
+      <c r="D468" s="4"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="C469" s="3"/>
+      <c r="D469" s="4"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="C470" s="3"/>
+      <c r="D470" s="4"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="C471" s="3"/>
+      <c r="D471" s="4"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="C472" s="3"/>
+      <c r="D472" s="4"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="C473" s="3"/>
+      <c r="D473" s="4"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="C474" s="3"/>
+      <c r="D474" s="4"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="C475" s="3"/>
+      <c r="D475" s="4"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="C476" s="3"/>
+      <c r="D476" s="4"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="C477" s="3"/>
+      <c r="D477" s="4"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="C478" s="3"/>
+      <c r="D478" s="4"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="C479" s="3"/>
+      <c r="D479" s="4"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="C480" s="3"/>
+      <c r="D480" s="4"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="C481" s="3"/>
+      <c r="D481" s="4"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="C482" s="3"/>
+      <c r="D482" s="4"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="C483" s="3"/>
+      <c r="D483" s="4"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="C484" s="3"/>
+      <c r="D484" s="4"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="C485" s="3"/>
+      <c r="D485" s="4"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="C486" s="3"/>
+      <c r="D486" s="4"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="C487" s="3"/>
+      <c r="D487" s="4"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="C488" s="3"/>
+      <c r="D488" s="4"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="C489" s="3"/>
+      <c r="D489" s="4"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="C490" s="3"/>
+      <c r="D490" s="4"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="C491" s="3"/>
+      <c r="D491" s="4"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="C492" s="3"/>
+      <c r="D492" s="4"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="C493" s="3"/>
+      <c r="D493" s="4"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="C494" s="3"/>
+      <c r="D494" s="4"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="C495" s="3"/>
+      <c r="D495" s="4"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="C496" s="3"/>
+      <c r="D496" s="4"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="C497" s="3"/>
+      <c r="D497" s="4"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="C498" s="3"/>
+      <c r="D498" s="4"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="C499" s="3"/>
+      <c r="D499" s="4"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="C500" s="3"/>
+      <c r="D500" s="4"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="C501" s="3"/>
+      <c r="D501" s="4"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="C502" s="3"/>
+      <c r="D502" s="4"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="C503" s="3"/>
+      <c r="D503" s="4"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="C504" s="3"/>
+      <c r="D504" s="4"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="C505" s="3"/>
+      <c r="D505" s="4"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="C506" s="3"/>
+      <c r="D506" s="4"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="C507" s="3"/>
+      <c r="D507" s="4"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="C508" s="3"/>
+      <c r="D508" s="4"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="C509" s="3"/>
+      <c r="D509" s="4"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="C510" s="3"/>
+      <c r="D510" s="4"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="C511" s="3"/>
+      <c r="D511" s="4"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="C512" s="3"/>
+      <c r="D512" s="4"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="C513" s="3"/>
+      <c r="D513" s="4"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="C514" s="3"/>
+      <c r="D514" s="4"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="C515" s="3"/>
+      <c r="D515" s="4"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="C516" s="3"/>
+      <c r="D516" s="4"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="C517" s="3"/>
+      <c r="D517" s="4"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="C518" s="3"/>
+      <c r="D518" s="4"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="C519" s="3"/>
+      <c r="D519" s="4"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="C520" s="3"/>
+      <c r="D520" s="4"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="C521" s="3"/>
+      <c r="D521" s="4"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="C522" s="3"/>
+      <c r="D522" s="4"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="C523" s="3"/>
+      <c r="D523" s="4"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="C524" s="3"/>
+      <c r="D524" s="4"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="C525" s="3"/>
+      <c r="D525" s="4"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="C526" s="3"/>
+      <c r="D526" s="4"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="C527" s="3"/>
+      <c r="D527" s="4"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="C528" s="3"/>
+      <c r="D528" s="4"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="C529" s="3"/>
+      <c r="D529" s="4"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="C530" s="3"/>
+      <c r="D530" s="4"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="C531" s="3"/>
+      <c r="D531" s="4"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="C532" s="3"/>
+      <c r="D532" s="4"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="C533" s="3"/>
+      <c r="D533" s="4"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="C534" s="3"/>
+      <c r="D534" s="4"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="C535" s="3"/>
+      <c r="D535" s="4"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="C536" s="3"/>
+      <c r="D536" s="4"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="C537" s="3"/>
+      <c r="D537" s="4"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="C538" s="3"/>
+      <c r="D538" s="4"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="C539" s="3"/>
+      <c r="D539" s="4"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="C540" s="3"/>
+      <c r="D540" s="4"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="C541" s="3"/>
+      <c r="D541" s="4"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="C542" s="3"/>
+      <c r="D542" s="4"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="C543" s="3"/>
+      <c r="D543" s="4"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="C544" s="3"/>
+      <c r="D544" s="4"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="C545" s="3"/>
+      <c r="D545" s="4"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="C546" s="3"/>
+      <c r="D546" s="4"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="C547" s="3"/>
+      <c r="D547" s="4"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="C548" s="3"/>
+      <c r="D548" s="4"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="C549" s="3"/>
+      <c r="D549" s="4"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="C550" s="3"/>
+      <c r="D550" s="4"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="C551" s="3"/>
+      <c r="D551" s="4"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="C552" s="3"/>
+      <c r="D552" s="4"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="C553" s="3"/>
+      <c r="D553" s="4"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="C554" s="3"/>
+      <c r="D554" s="4"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="C555" s="3"/>
+      <c r="D555" s="4"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="C556" s="3"/>
+      <c r="D556" s="4"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="C557" s="3"/>
+      <c r="D557" s="4"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="C558" s="3"/>
+      <c r="D558" s="4"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="C559" s="3"/>
+      <c r="D559" s="4"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="C560" s="3"/>
+      <c r="D560" s="4"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="C561" s="3"/>
+      <c r="D561" s="4"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="C562" s="3"/>
+      <c r="D562" s="4"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="C563" s="3"/>
+      <c r="D563" s="4"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="C564" s="3"/>
+      <c r="D564" s="4"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="C565" s="3"/>
+      <c r="D565" s="4"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="C566" s="3"/>
+      <c r="D566" s="4"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="C567" s="3"/>
+      <c r="D567" s="4"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="C568" s="3"/>
+      <c r="D568" s="4"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="C569" s="3"/>
+      <c r="D569" s="4"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="C570" s="3"/>
+      <c r="D570" s="4"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="C571" s="3"/>
+      <c r="D571" s="4"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="C572" s="3"/>
+      <c r="D572" s="4"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="C573" s="3"/>
+      <c r="D573" s="4"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="C574" s="3"/>
+      <c r="D574" s="4"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="C575" s="3"/>
+      <c r="D575" s="4"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="C576" s="3"/>
+      <c r="D576" s="4"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="C577" s="3"/>
+      <c r="D577" s="4"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="C578" s="3"/>
+      <c r="D578" s="4"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="C579" s="3"/>
+      <c r="D579" s="4"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="C580" s="3"/>
+      <c r="D580" s="4"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="C581" s="3"/>
+      <c r="D581" s="4"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="C582" s="3"/>
+      <c r="D582" s="4"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="C583" s="3"/>
+      <c r="D583" s="4"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="C584" s="3"/>
+      <c r="D584" s="4"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="C585" s="3"/>
+      <c r="D585" s="4"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="C586" s="3"/>
+      <c r="D586" s="4"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="C587" s="3"/>
+      <c r="D587" s="4"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="C588" s="3"/>
+      <c r="D588" s="4"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="C589" s="3"/>
+      <c r="D589" s="4"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="C590" s="3"/>
+      <c r="D590" s="4"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="C591" s="3"/>
+      <c r="D591" s="4"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="C592" s="3"/>
+      <c r="D592" s="4"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="C593" s="3"/>
+      <c r="D593" s="4"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="C594" s="3"/>
+      <c r="D594" s="4"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="C595" s="3"/>
+      <c r="D595" s="4"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="C596" s="3"/>
+      <c r="D596" s="4"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="C597" s="3"/>
+      <c r="D597" s="4"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="C598" s="3"/>
+      <c r="D598" s="4"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="C599" s="3"/>
+      <c r="D599" s="4"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="C600" s="3"/>
+      <c r="D600" s="4"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="C601" s="3"/>
+      <c r="D601" s="4"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="C602" s="3"/>
+      <c r="D602" s="4"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="C603" s="3"/>
+      <c r="D603" s="4"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="C604" s="3"/>
+      <c r="D604" s="4"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="C605" s="3"/>
+      <c r="D605" s="4"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="C606" s="3"/>
+      <c r="D606" s="4"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="C607" s="3"/>
+      <c r="D607" s="4"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="C608" s="3"/>
+      <c r="D608" s="4"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="C609" s="3"/>
+      <c r="D609" s="4"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="C610" s="3"/>
+      <c r="D610" s="4"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="C611" s="3"/>
+      <c r="D611" s="4"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="C612" s="3"/>
+      <c r="D612" s="4"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="C613" s="3"/>
+      <c r="D613" s="4"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="C614" s="3"/>
+      <c r="D614" s="4"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="C615" s="3"/>
+      <c r="D615" s="4"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="C616" s="3"/>
+      <c r="D616" s="4"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="C617" s="3"/>
+      <c r="D617" s="4"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="C618" s="3"/>
+      <c r="D618" s="4"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="C619" s="3"/>
+      <c r="D619" s="4"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="C620" s="3"/>
+      <c r="D620" s="4"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="C621" s="3"/>
+      <c r="D621" s="4"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="C622" s="3"/>
+      <c r="D622" s="6"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="C623" s="3"/>
+      <c r="D623" s="6"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="C624" s="3"/>
+      <c r="D624" s="6"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="C625" s="3"/>
+      <c r="D625" s="6"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="C626" s="3"/>
+      <c r="D626" s="6"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="C627" s="3"/>
+      <c r="D627" s="6"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="C628" s="3"/>
+      <c r="D628" s="6"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="C629" s="3"/>
+      <c r="D629" s="6"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="C630" s="3"/>
+      <c r="D630" s="6"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="C631" s="3"/>
+      <c r="D631" s="6"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="C632" s="3"/>
+      <c r="D632" s="6"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="C633" s="3"/>
+      <c r="D633" s="6"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="C634" s="3"/>
+      <c r="D634" s="6"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="C635" s="3"/>
+      <c r="D635" s="6"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="C636" s="3"/>
+      <c r="D636" s="6"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="C637" s="3"/>
+      <c r="D637" s="6"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="C638" s="3"/>
+      <c r="D638" s="6"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="C639" s="3"/>
+      <c r="D639" s="6"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="C640" s="3"/>
+      <c r="D640" s="6"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="C641" s="3"/>
+      <c r="D641" s="6"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="C642" s="3"/>
+      <c r="D642" s="6"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="C643" s="3"/>
+      <c r="D643" s="6"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="C644" s="3"/>
+      <c r="D644" s="6"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="C645" s="3"/>
+      <c r="D645" s="6"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="C646" s="3"/>
+      <c r="D646" s="6"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="C647" s="3"/>
+      <c r="D647" s="6"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="C648" s="3"/>
+      <c r="D648" s="6"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="C649" s="3"/>
+      <c r="D649" s="6"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="C650" s="3"/>
+      <c r="D650" s="6"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="C651" s="3"/>
+      <c r="D651" s="6"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="C652" s="3"/>
+      <c r="D652" s="6"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="C653" s="3"/>
+      <c r="D653" s="6"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="C654" s="3"/>
+      <c r="D654" s="6"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="C655" s="3"/>
+      <c r="D655" s="6"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="C656" s="3"/>
+      <c r="D656" s="6"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="C657" s="3"/>
+      <c r="D657" s="6"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="C658" s="3"/>
+      <c r="D658" s="6"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="C659" s="3"/>
+      <c r="D659" s="6"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="C660" s="3"/>
+      <c r="D660" s="6"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="C661" s="3"/>
+      <c r="D661" s="6"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="C662" s="3"/>
+      <c r="D662" s="6"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="C663" s="3"/>
+      <c r="D663" s="6"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="C664" s="3"/>
+      <c r="D664" s="6"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="C665" s="3"/>
+      <c r="D665" s="6"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="C666" s="3"/>
+      <c r="D666" s="6"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="C667" s="3"/>
+      <c r="D667" s="6"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="C668" s="3"/>
+      <c r="D668" s="6"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="C669" s="3"/>
+      <c r="D669" s="6"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="C670" s="3"/>
+      <c r="D670" s="6"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="C671" s="3"/>
+      <c r="D671" s="6"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="C672" s="3"/>
+      <c r="D672" s="6"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="C673" s="3"/>
+      <c r="D673" s="6"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="C674" s="3"/>
+      <c r="D674" s="6"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="C675" s="3"/>
+      <c r="D675" s="6"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="C676" s="3"/>
+      <c r="D676" s="6"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="C677" s="3"/>
+      <c r="D677" s="6"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="C678" s="3"/>
+      <c r="D678" s="6"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="C679" s="3"/>
+      <c r="D679" s="6"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="C680" s="3"/>
+      <c r="D680" s="6"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="C681" s="3"/>
+      <c r="D681" s="6"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="C682" s="3"/>
+      <c r="D682" s="6"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="C683" s="3"/>
+      <c r="D683" s="6"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="C684" s="3"/>
+      <c r="D684" s="6"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="C685" s="3"/>
+      <c r="D685" s="6"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="C686" s="3"/>
+      <c r="D686" s="6"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="C687" s="3"/>
+      <c r="D687" s="6"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="C688" s="3"/>
+      <c r="D688" s="6"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="C689" s="3"/>
+      <c r="D689" s="6"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="C690" s="3"/>
+      <c r="D690" s="6"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="C691" s="3"/>
+      <c r="D691" s="6"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="C692" s="3"/>
+      <c r="D692" s="6"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="C693" s="3"/>
+      <c r="D693" s="6"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="C694" s="3"/>
+      <c r="D694" s="6"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="C695" s="3"/>
+      <c r="D695" s="6"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="C696" s="3"/>
+      <c r="D696" s="6"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="C697" s="3"/>
+      <c r="D697" s="6"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="C698" s="3"/>
+      <c r="D698" s="6"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="C699" s="3"/>
+      <c r="D699" s="6"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="C700" s="3"/>
+      <c r="D700" s="6"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="C701" s="3"/>
+      <c r="D701" s="6"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="C702" s="3"/>
+      <c r="D702" s="6"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="C703" s="3"/>
+      <c r="D703" s="6"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="C704" s="3"/>
+      <c r="D704" s="6"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="C705" s="3"/>
+      <c r="D705" s="6"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="C706" s="3"/>
+      <c r="D706" s="6"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="C707" s="3"/>
+      <c r="D707" s="6"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="C708" s="3"/>
+      <c r="D708" s="6"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="C709" s="3"/>
+      <c r="D709" s="6"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="C710" s="3"/>
+      <c r="D710" s="6"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="C711" s="3"/>
+      <c r="D711" s="6"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="C712" s="3"/>
+      <c r="D712" s="6"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="C713" s="3"/>
+      <c r="D713" s="6"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="C714" s="3"/>
+      <c r="D714" s="6"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="C715" s="3"/>
+      <c r="D715" s="6"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="C716" s="3"/>
+      <c r="D716" s="6"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="C717" s="3"/>
+      <c r="D717" s="6"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="C718" s="3"/>
+      <c r="D718" s="6"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="C719" s="3"/>
+      <c r="D719" s="6"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="C720" s="3"/>
+      <c r="D720" s="6"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="C721" s="3"/>
+      <c r="D721" s="6"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="C722" s="3"/>
+      <c r="D722" s="6"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="C723" s="3"/>
+      <c r="D723" s="6"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="C724" s="3"/>
+      <c r="D724" s="6"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="C725" s="3"/>
+      <c r="D725" s="6"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="C726" s="3"/>
+      <c r="D726" s="6"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="C727" s="3"/>
+      <c r="D727" s="6"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="C728" s="3"/>
+      <c r="D728" s="6"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="C729" s="3"/>
+      <c r="D729" s="6"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="C730" s="3"/>
+      <c r="D730" s="6"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="C731" s="3"/>
+      <c r="D731" s="6"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="C732" s="3"/>
+      <c r="D732" s="6"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="C733" s="3"/>
+      <c r="D733" s="6"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="C734" s="3"/>
+      <c r="D734" s="6"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="C735" s="3"/>
+      <c r="D735" s="6"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="C736" s="3"/>
+      <c r="D736" s="6"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="C737" s="3"/>
+      <c r="D737" s="6"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="C738" s="3"/>
+      <c r="D738" s="6"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="C739" s="3"/>
+      <c r="D739" s="6"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="C740" s="3"/>
+      <c r="D740" s="6"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="C741" s="3"/>
+      <c r="D741" s="6"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="C742" s="3"/>
+      <c r="D742" s="6"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="C743" s="3"/>
+      <c r="D743" s="6"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="C744" s="3"/>
+      <c r="D744" s="6"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="C745" s="3"/>
+      <c r="D745" s="6"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="C746" s="3"/>
+      <c r="D746" s="6"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="C747" s="3"/>
+      <c r="D747" s="6"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="C748" s="3"/>
+      <c r="D748" s="6"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="C749" s="3"/>
+      <c r="D749" s="6"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="C750" s="3"/>
+      <c r="D750" s="6"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="C751" s="3"/>
+      <c r="D751" s="6"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="C752" s="3"/>
+      <c r="D752" s="6"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="C753" s="3"/>
+      <c r="D753" s="6"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="C754" s="3"/>
+      <c r="D754" s="6"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="C755" s="3"/>
+      <c r="D755" s="6"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="C756" s="3"/>
+      <c r="D756" s="6"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="C757" s="3"/>
+      <c r="D757" s="6"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="C758" s="3"/>
+      <c r="D758" s="6"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="C759" s="3"/>
+      <c r="D759" s="6"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="C760" s="3"/>
+      <c r="D760" s="6"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="C761" s="3"/>
+      <c r="D761" s="6"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="C762" s="3"/>
+      <c r="D762" s="6"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="C763" s="3"/>
+      <c r="D763" s="6"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="C764" s="3"/>
+      <c r="D764" s="6"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="C765" s="3"/>
+      <c r="D765" s="6"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="C766" s="3"/>
+      <c r="D766" s="6"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="C767" s="3"/>
+      <c r="D767" s="6"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="C768" s="3"/>
+      <c r="D768" s="6"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="C769" s="3"/>
+      <c r="D769" s="6"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="C770" s="3"/>
+      <c r="D770" s="6"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="C771" s="3"/>
+      <c r="D771" s="6"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="C772" s="3"/>
+      <c r="D772" s="6"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="C773" s="3"/>
+      <c r="D773" s="6"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="C774" s="3"/>
+      <c r="D774" s="6"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="C775" s="3"/>
+      <c r="D775" s="6"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="C776" s="3"/>
+      <c r="D776" s="6"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="C777" s="3"/>
+      <c r="D777" s="6"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="C778" s="3"/>
+      <c r="D778" s="6"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="C779" s="3"/>
+      <c r="D779" s="6"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="C780" s="3"/>
+      <c r="D780" s="6"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="C781" s="3"/>
+      <c r="D781" s="6"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="C782" s="3"/>
+      <c r="D782" s="6"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="C783" s="3"/>
+      <c r="D783" s="6"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="C784" s="3"/>
+      <c r="D784" s="6"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="C785" s="3"/>
+      <c r="D785" s="6"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="C786" s="3"/>
+      <c r="D786" s="6"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="C787" s="3"/>
+      <c r="D787" s="6"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="C788" s="3"/>
+      <c r="D788" s="6"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="C789" s="3"/>
+      <c r="D789" s="6"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="C790" s="3"/>
+      <c r="D790" s="6"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="C791" s="3"/>
+      <c r="D791" s="6"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="C792" s="3"/>
+      <c r="D792" s="6"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="C793" s="3"/>
+      <c r="D793" s="6"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="C794" s="3"/>
+      <c r="D794" s="6"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="C795" s="3"/>
+      <c r="D795" s="6"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="C796" s="3"/>
+      <c r="D796" s="6"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="C797" s="3"/>
+      <c r="D797" s="6"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="C798" s="3"/>
+      <c r="D798" s="6"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="C799" s="3"/>
+      <c r="D799" s="6"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="C800" s="3"/>
+      <c r="D800" s="6"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="C801" s="3"/>
+      <c r="D801" s="6"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="C802" s="3"/>
+      <c r="D802" s="6"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="C803" s="3"/>
+      <c r="D803" s="6"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="C804" s="3"/>
+      <c r="D804" s="6"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="C805" s="3"/>
+      <c r="D805" s="6"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="C806" s="3"/>
+      <c r="D806" s="6"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="C807" s="3"/>
+      <c r="D807" s="6"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="C808" s="3"/>
+      <c r="D808" s="6"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="C809" s="3"/>
+      <c r="D809" s="6"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="C810" s="3"/>
+      <c r="D810" s="6"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="C811" s="3"/>
+      <c r="D811" s="6"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="C812" s="3"/>
+      <c r="D812" s="6"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="C813" s="3"/>
+      <c r="D813" s="6"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="C814" s="3"/>
+      <c r="D814" s="6"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="C815" s="3"/>
+      <c r="D815" s="6"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="C816" s="3"/>
+      <c r="D816" s="6"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="C817" s="3"/>
+      <c r="D817" s="6"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="C818" s="3"/>
+      <c r="D818" s="6"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="C819" s="3"/>
+      <c r="D819" s="6"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="C820" s="3"/>
+      <c r="D820" s="6"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="C821" s="3"/>
+      <c r="D821" s="6"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="C822" s="3"/>
+      <c r="D822" s="6"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="C823" s="3"/>
+      <c r="D823" s="6"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="C824" s="3"/>
+      <c r="D824" s="6"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="C825" s="3"/>
+      <c r="D825" s="6"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="C826" s="3"/>
+      <c r="D826" s="6"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="C827" s="3"/>
+      <c r="D827" s="6"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="C828" s="3"/>
+      <c r="D828" s="6"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="C829" s="3"/>
+      <c r="D829" s="6"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="C830" s="3"/>
+      <c r="D830" s="6"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="C831" s="3"/>
+      <c r="D831" s="6"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="C832" s="3"/>
+      <c r="D832" s="6"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="C833" s="3"/>
+      <c r="D833" s="6"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="C834" s="3"/>
+      <c r="D834" s="6"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="C835" s="3"/>
+      <c r="D835" s="6"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="C836" s="3"/>
+      <c r="D836" s="6"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="C837" s="3"/>
+      <c r="D837" s="6"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="C838" s="3"/>
+      <c r="D838" s="6"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="C839" s="3"/>
+      <c r="D839" s="6"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="C840" s="3"/>
+      <c r="D840" s="6"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="C841" s="3"/>
+      <c r="D841" s="6"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="C842" s="3"/>
+      <c r="D842" s="6"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="C843" s="3"/>
+      <c r="D843" s="6"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="C844" s="3"/>
+      <c r="D844" s="6"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="C845" s="3"/>
+      <c r="D845" s="6"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="C846" s="3"/>
+      <c r="D846" s="6"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="C847" s="3"/>
+      <c r="D847" s="6"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="C848" s="3"/>
+      <c r="D848" s="6"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="C849" s="3"/>
+      <c r="D849" s="6"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="C850" s="3"/>
+      <c r="D850" s="6"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="C851" s="3"/>
+      <c r="D851" s="6"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="C852" s="3"/>
+      <c r="D852" s="6"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="C853" s="3"/>
+      <c r="D853" s="6"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="C854" s="3"/>
+      <c r="D854" s="6"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="C855" s="3"/>
+      <c r="D855" s="6"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="C856" s="3"/>
+      <c r="D856" s="6"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="C857" s="3"/>
+      <c r="D857" s="6"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="C858" s="3"/>
+      <c r="D858" s="6"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="C859" s="3"/>
+      <c r="D859" s="6"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="C860" s="3"/>
+      <c r="D860" s="6"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="C861" s="3"/>
+      <c r="D861" s="6"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="C862" s="3"/>
+      <c r="D862" s="6"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="C863" s="3"/>
+      <c r="D863" s="6"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="C864" s="3"/>
+      <c r="D864" s="6"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="C865" s="3"/>
+      <c r="D865" s="6"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="C866" s="3"/>
+      <c r="D866" s="6"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="C867" s="3"/>
+      <c r="D867" s="6"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="C868" s="3"/>
+      <c r="D868" s="6"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="C869" s="3"/>
+      <c r="D869" s="6"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="C870" s="3"/>
+      <c r="D870" s="6"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="C871" s="3"/>
+      <c r="D871" s="6"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="C872" s="3"/>
+      <c r="D872" s="6"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="C873" s="3"/>
+      <c r="D873" s="6"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="C874" s="3"/>
+      <c r="D874" s="6"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="C875" s="3"/>
+      <c r="D875" s="6"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="C876" s="3"/>
+      <c r="D876" s="6"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="C877" s="3"/>
+      <c r="D877" s="6"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="C878" s="3"/>
+      <c r="D878" s="6"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="C879" s="3"/>
+      <c r="D879" s="6"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="C880" s="3"/>
+      <c r="D880" s="6"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="C881" s="3"/>
+      <c r="D881" s="6"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="C882" s="3"/>
+      <c r="D882" s="6"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="C883" s="3"/>
+      <c r="D883" s="6"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="C884" s="3"/>
+      <c r="D884" s="6"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="C885" s="3"/>
+      <c r="D885" s="6"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="C886" s="3"/>
+      <c r="D886" s="6"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="C887" s="3"/>
+      <c r="D887" s="6"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="C888" s="3"/>
+      <c r="D888" s="6"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="C889" s="3"/>
+      <c r="D889" s="6"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="C890" s="3"/>
+      <c r="D890" s="6"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="C891" s="3"/>
+      <c r="D891" s="6"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="C892" s="3"/>
+      <c r="D892" s="6"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="C893" s="3"/>
+      <c r="D893" s="6"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="C894" s="3"/>
+      <c r="D894" s="6"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="C895" s="3"/>
+      <c r="D895" s="6"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="C896" s="3"/>
+      <c r="D896" s="6"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="C897" s="3"/>
+      <c r="D897" s="6"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="C898" s="3"/>
+      <c r="D898" s="6"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="C899" s="3"/>
+      <c r="D899" s="6"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="C900" s="3"/>
+      <c r="D900" s="6"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="C901" s="3"/>
+      <c r="D901" s="6"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="C902" s="3"/>
+      <c r="D902" s="6"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="C903" s="3"/>
+      <c r="D903" s="6"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="C904" s="3"/>
+      <c r="D904" s="6"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="C905" s="3"/>
+      <c r="D905" s="6"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="C906" s="3"/>
+      <c r="D906" s="6"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="C907" s="3"/>
+      <c r="D907" s="6"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="C908" s="3"/>
+      <c r="D908" s="6"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="C909" s="3"/>
+      <c r="D909" s="6"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="C910" s="3"/>
+      <c r="D910" s="6"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="C911" s="3"/>
+      <c r="D911" s="6"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="C912" s="3"/>
+      <c r="D912" s="6"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="C913" s="3"/>
+      <c r="D913" s="6"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="C914" s="3"/>
+      <c r="D914" s="6"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="C915" s="3"/>
+      <c r="D915" s="6"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="C916" s="3"/>
+      <c r="D916" s="6"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="C917" s="3"/>
+      <c r="D917" s="6"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="C918" s="3"/>
+      <c r="D918" s="6"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="C919" s="3"/>
+      <c r="D919" s="6"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="C920" s="3"/>
+      <c r="D920" s="6"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="C921" s="3"/>
+      <c r="D921" s="6"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="C922" s="3"/>
+      <c r="D922" s="6"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="C923" s="3"/>
+      <c r="D923" s="6"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="C924" s="3"/>
+      <c r="D924" s="6"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="C925" s="3"/>
+      <c r="D925" s="6"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="C926" s="3"/>
+      <c r="D926" s="6"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="C927" s="3"/>
+      <c r="D927" s="6"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="C928" s="3"/>
+      <c r="D928" s="6"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="C929" s="3"/>
+      <c r="D929" s="6"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="C930" s="3"/>
+      <c r="D930" s="6"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="C931" s="3"/>
+      <c r="D931" s="6"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="C932" s="3"/>
+      <c r="D932" s="6"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="C933" s="3"/>
+      <c r="D933" s="6"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="C934" s="3"/>
+      <c r="D934" s="6"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="C935" s="3"/>
+      <c r="D935" s="6"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="C936" s="3"/>
+      <c r="D936" s="6"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="C937" s="3"/>
+      <c r="D937" s="6"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="C938" s="3"/>
+      <c r="D938" s="6"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="C939" s="3"/>
+      <c r="D939" s="6"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="C940" s="3"/>
+      <c r="D940" s="6"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="C941" s="3"/>
+      <c r="D941" s="6"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="C942" s="3"/>
+      <c r="D942" s="6"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="C943" s="3"/>
+      <c r="D943" s="6"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="C944" s="3"/>
+      <c r="D944" s="6"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="C945" s="3"/>
+      <c r="D945" s="6"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="C946" s="3"/>
+      <c r="D946" s="6"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="C947" s="3"/>
+      <c r="D947" s="6"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="C948" s="3"/>
+      <c r="D948" s="6"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="C949" s="3"/>
+      <c r="D949" s="6"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="C950" s="3"/>
+      <c r="D950" s="6"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="C951" s="3"/>
+      <c r="D951" s="6"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="C952" s="3"/>
+      <c r="D952" s="6"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="C953" s="3"/>
+      <c r="D953" s="6"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="C954" s="3"/>
+      <c r="D954" s="6"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="C955" s="3"/>
+      <c r="D955" s="6"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="C956" s="3"/>
+      <c r="D956" s="6"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="C957" s="3"/>
+      <c r="D957" s="6"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="C958" s="3"/>
+      <c r="D958" s="6"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="C959" s="3"/>
+      <c r="D959" s="6"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="C960" s="3"/>
+      <c r="D960" s="6"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="C961" s="3"/>
+      <c r="D961" s="6"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="C962" s="3"/>
+      <c r="D962" s="6"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="C963" s="3"/>
+      <c r="D963" s="6"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="C964" s="3"/>
+      <c r="D964" s="6"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="C965" s="3"/>
+      <c r="D965" s="6"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="C966" s="3"/>
+      <c r="D966" s="6"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="C967" s="3"/>
+      <c r="D967" s="6"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="C968" s="3"/>
+      <c r="D968" s="6"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="C969" s="3"/>
+      <c r="D969" s="6"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="C970" s="3"/>
+      <c r="D970" s="6"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="C971" s="3"/>
+      <c r="D971" s="6"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="C972" s="3"/>
+      <c r="D972" s="6"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="C973" s="3"/>
+      <c r="D973" s="6"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="C974" s="3"/>
+      <c r="D974" s="6"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="C975" s="3"/>
+      <c r="D975" s="6"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="C976" s="3"/>
+      <c r="D976" s="6"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="C977" s="3"/>
+      <c r="D977" s="6"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="C978" s="3"/>
+      <c r="D978" s="6"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="C979" s="3"/>
+      <c r="D979" s="6"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="C980" s="3"/>
+      <c r="D980" s="6"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="C981" s="3"/>
+      <c r="D981" s="6"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="C982" s="3"/>
+      <c r="D982" s="6"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="C983" s="3"/>
+      <c r="D983" s="6"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="C984" s="3"/>
+      <c r="D984" s="6"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="C985" s="3"/>
+      <c r="D985" s="6"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="C986" s="3"/>
+      <c r="D986" s="6"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="C987" s="3"/>
+      <c r="D987" s="6"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="C988" s="3"/>
+      <c r="D988" s="6"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="C989" s="3"/>
+      <c r="D989" s="6"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="C990" s="3"/>
+      <c r="D990" s="6"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="C991" s="3"/>
+      <c r="D991" s="6"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="C992" s="3"/>
+      <c r="D992" s="6"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="C993" s="3"/>
+      <c r="D993" s="6"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="C994" s="3"/>
+      <c r="D994" s="6"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
-      <c r="C995" s="3"/>
+      <c r="D995" s="6"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
-      <c r="C996" s="3"/>
+      <c r="D996" s="6"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
-      <c r="C997" s="3"/>
+      <c r="D997" s="6"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
-      <c r="C998" s="3"/>
+      <c r="D998" s="6"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
-      <c r="C999" s="3"/>
+      <c r="D999" s="6"/>
     </row>
     <row r="1000" ht="15.75" customHeight="1">
-      <c r="C1000" s="3"/>
+      <c r="D1000" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1000">
+  <conditionalFormatting sqref="D1:D1000">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C1))&gt;0</formula>
+      <formula>LEN(TRIM(D1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D622:D1000">
       <formula1>'Hoja 2'!$A$2:$A$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D621">
+      <formula1>'Hoja 2'!$A$2:$A$15</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -3631,72 +3652,80 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>

</xml_diff>